<commit_message>
Make the scraping stuff more modular
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylej\Documents\UiPath\MovieSearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabh\Documents\UiPath\MovieSearch2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F2F457-960C-4BD1-BF91-36369BE656A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C171C848-35F3-4804-9192-81C179FF602F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="878" yWindow="1628" windowWidth="15390" windowHeight="9532" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11325" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="200">
   <si>
     <t>Movie Name</t>
   </si>
@@ -81,12 +81,6 @@
     <t>George Dewey / Dan Levine / Michael Riley McGrath / Josh McLaglen / Mary McLaglen</t>
   </si>
   <si>
-    <t>Dan Cohen / Rand Geiger</t>
-  </si>
-  <si>
-    <t>Shawn Levy</t>
-  </si>
-  <si>
     <t>The Suicide Squad</t>
   </si>
   <si>
@@ -99,12 +93,6 @@
     <t>Walter Hamada / Nikolas Korda / Deborah Snyder / Zack Snyder / Richard Suckle / Chantal Nong Vo</t>
   </si>
   <si>
-    <t>Arianne Benedetti / Simon Hatt / Lars P. Winther</t>
-  </si>
-  <si>
-    <t>James Gunn</t>
-  </si>
-  <si>
     <t>Candyman</t>
   </si>
   <si>
@@ -123,12 +111,6 @@
     <t>Shauna Bryan / Jason Cloth / Aaron L. Gilbert / David Kern</t>
   </si>
   <si>
-    <t>Brittany Klesic</t>
-  </si>
-  <si>
-    <t>Nia DaCosta</t>
-  </si>
-  <si>
     <t>PAW Patrol: The Movie</t>
   </si>
   <si>
@@ -144,12 +126,6 @@
     <t>Adam Beder / Ronnen Harary / Zai Ortiz / Peter Schlessel</t>
   </si>
   <si>
-    <t>Laura Clunie / Amanda Morgan Palmer / Toni Stevens / Lauren Talbot / Laurence Vacher</t>
-  </si>
-  <si>
-    <t>Cal Brunker</t>
-  </si>
-  <si>
     <t>Don't Breathe 2</t>
   </si>
   <si>
@@ -165,12 +141,6 @@
     <t>Joseph Drake / Rick Jacobson / Nathan Kahane / Stephen Lang / Andrew Pfeffer / Erin Westerman</t>
   </si>
   <si>
-    <t>Romel Adam / Brady Fujikawa / Kelli Konop / Dave Krieger / Rodo Sayagues</t>
-  </si>
-  <si>
-    <t>Rodo Sayagues</t>
-  </si>
-  <si>
     <t>Respect</t>
   </si>
   <si>
@@ -201,12 +171,6 @@
     <t>Andrei Boncea / Dragos Buliga / Christa Campbell / Luke Daniels / Boaz Davidson / Claiton Fernandes / Vladimir Fernandes / Jeffrey Greenstein / Lati Grobman / Avi Lerner / Balan Melarkode / Euzebio Munhoz Jr. / Daniel Negret / Trevor Short / Kyle Stroud / Gareth West / Simon Williams / Bruno Wu / Jonathan Yunger</t>
   </si>
   <si>
-    <t>Ekaterina Baker / Valentin Dimitrov / Bernard Mazauric / Gabriel Popescu / Lonnie Ramati / Regina Seifert</t>
-  </si>
-  <si>
-    <t>Martin Campbell</t>
-  </si>
-  <si>
     <t>The Night House</t>
   </si>
   <si>
@@ -222,12 +186,6 @@
     <t>David Bruckner / François Callens / Ben Collins / Tara Finegan / George Paaswell / Luke Piotrowski / Sébastien Raybaud / Laura Wilson</t>
   </si>
   <si>
-    <t>Alexander Norton / Todd Williams</t>
-  </si>
-  <si>
-    <t>David Bruckner</t>
-  </si>
-  <si>
     <t>Reminiscence</t>
   </si>
   <si>
@@ -240,9 +198,6 @@
     <t>Elishia Holmes / D. Scott Lumpkin / Athena Wickham</t>
   </si>
   <si>
-    <t>Lisa Joy</t>
-  </si>
-  <si>
     <t>An Egg Rescue</t>
   </si>
   <si>
@@ -255,12 +210,6 @@
     <t>Mineko Mori / Jd Segura Jr. / Cleo Segura Sherrel / Carlos Zepeda</t>
   </si>
   <si>
-    <t>Paula Báez / Regina Diaz Torre / Estefanía Franco / Andy Rodríguez / Janine Hernández Vidals / María Sol Yépez</t>
-  </si>
-  <si>
-    <t>Gabriel Riva Palacio Alatriste / Rodolfo Riva Palacio Alatriste</t>
-  </si>
-  <si>
     <t>Flag Day</t>
   </si>
   <si>
@@ -279,12 +228,6 @@
     <t>Christelle Conan / Lawrence M. Kopeikin / Phyllis Laing / Thorsten Schumacher / Peter Touche / Devan Towers / John Wildermuth</t>
   </si>
   <si>
-    <t>Mary Aloe / Gillian Hormel / Mark Montague / Dana Mulligan / John Ira Palmer / Matt Palmieri / Joseph Sacks / Katheryn Winnick</t>
-  </si>
-  <si>
-    <t>Sean Penn</t>
-  </si>
-  <si>
     <t>The Lost Leonardo</t>
   </si>
   <si>
@@ -300,12 +243,6 @@
     <t>Oli Harbottle / Mark Mitten / Ken Pelletier / Vijay Vaidyanathan</t>
   </si>
   <si>
-    <t>Duska Zagorac</t>
-  </si>
-  <si>
-    <t>Andreas Koefoed</t>
-  </si>
-  <si>
     <t>Raging Fire</t>
   </si>
   <si>
@@ -318,18 +255,12 @@
     <t>Albert Yeung</t>
   </si>
   <si>
-    <t>Benny Chan</t>
-  </si>
-  <si>
     <t>Escape from Mogadishu</t>
   </si>
   <si>
     <t>Seong-min Jo / Jung-min Kim / Su-jin Park</t>
   </si>
   <si>
-    <t>Seung-wan Ryoo</t>
-  </si>
-  <si>
     <t>Together</t>
   </si>
   <si>
@@ -339,12 +270,6 @@
     <t>Rose Garnett / Gaynor Holmes / Dennis Kelly</t>
   </si>
   <si>
-    <t>Robert How</t>
-  </si>
-  <si>
-    <t>Stephen Daldry / Justin Martin</t>
-  </si>
-  <si>
     <t>Swan Song</t>
   </si>
   <si>
@@ -360,12 +285,6 @@
     <t>Jay Michael Fraley / Drew Sklar / Rhet Topham</t>
   </si>
   <si>
-    <t>Kenneth Altman</t>
-  </si>
-  <si>
-    <t>Todd Stephens</t>
-  </si>
-  <si>
     <t>Demonic</t>
   </si>
   <si>
@@ -381,21 +300,12 @@
     <t>Alastair Burlingham / Charlie Dombek / Viktor Muller / Miguel Palos / Steven St. Arnaud</t>
   </si>
   <si>
-    <t>Neill Blomkamp</t>
-  </si>
-  <si>
     <t>On Broadway</t>
   </si>
   <si>
     <t>Kino Lorber</t>
   </si>
   <si>
-    <t>Joel Goodman</t>
-  </si>
-  <si>
-    <t>Oren Jacoby</t>
-  </si>
-  <si>
     <t>Ema</t>
   </si>
   <si>
@@ -408,12 +318,6 @@
     <t>Amelia Granger / Ben Knight</t>
   </si>
   <si>
-    <t>Thea Paulett / Katherine Pomfret / Jo Wallett</t>
-  </si>
-  <si>
-    <t>Autumn de Wilde</t>
-  </si>
-  <si>
     <t>Death Rider in the House of Vampires</t>
   </si>
   <si>
@@ -429,12 +333,6 @@
     <t>Glenn Danzig / Brian Perera / Yvonne Perera</t>
   </si>
   <si>
-    <t>Charles Arthur Berg</t>
-  </si>
-  <si>
-    <t>Glenn Danzig</t>
-  </si>
-  <si>
     <t>Confetti</t>
   </si>
   <si>
@@ -447,12 +345,6 @@
     <t>Oliver Edwards / Joe Oppenheimer / Andrew Taylor / Lee Thomas / David M. Thompson</t>
   </si>
   <si>
-    <t>May Chu / Nick Jones</t>
-  </si>
-  <si>
-    <t>Debbie Isitt</t>
-  </si>
-  <si>
     <t>Cryptozoo</t>
   </si>
   <si>
@@ -462,9 +354,6 @@
     <t>Dexter Braff / Gail Flannigan / Drew Sykes</t>
   </si>
   <si>
-    <t>Dash Shaw</t>
-  </si>
-  <si>
     <t>Ma Belle, My Beauty</t>
   </si>
   <si>
@@ -477,9 +366,6 @@
     <t>Zaferhan Yumru</t>
   </si>
   <si>
-    <t>Marion Hill</t>
-  </si>
-  <si>
     <t>John and the Hole</t>
   </si>
   <si>
@@ -489,12 +375,6 @@
     <t>P. Jennifer Dana / Phil Hoelting / Ross Jacobson / Tony Pachella / Mark Roberts / Pascual Sisto / Marco Vicini</t>
   </si>
   <si>
-    <t>Rowan Riley / Sam Slater / Fernando Tsai</t>
-  </si>
-  <si>
-    <t>Pascual Sisto</t>
-  </si>
-  <si>
     <t>Even in Dreams</t>
   </si>
   <si>
@@ -510,12 +390,6 @@
     <t>Robbie Bryan / Steven D'Alo / Pete D'Arruda / Sessalie Daun / Lucas A. Ferrara / Jacob Joseph / Savannah Ostler / Theodore Stump</t>
   </si>
   <si>
-    <t>Alison Arngrim / Mario DeAngelis / Cal Nguyen / Monica Moore Smith</t>
-  </si>
-  <si>
-    <t>Savannah Ostler</t>
-  </si>
-  <si>
     <t>Bring Your Own Brigade</t>
   </si>
   <si>
@@ -528,12 +402,6 @@
     <t>Bill Benenson / Laurie Benenson / Michael Bloom / Geralyn White Dreyfous / Kathryn Everett / Ryan Heller / Tony Hsieh / Jena King / Lisa Leingang / Adam Lewis / Melony Lewis / Bryn Mooser / Regina K. Scully / Lynda Weinman / Jamie Wolf / Maria Zuckerman</t>
   </si>
   <si>
-    <t>Jennie Bedusa / Christine Connor / Sam Kahn</t>
-  </si>
-  <si>
-    <t>Lucy Walker</t>
-  </si>
-  <si>
     <t>The Meaning of Hitler</t>
   </si>
   <si>
@@ -543,9 +411,6 @@
     <t>Anthony Dobkin / Marie Therese Guirgis / Jeffrey Lurie</t>
   </si>
   <si>
-    <t>Petra Epperlein / Michael Tucker</t>
-  </si>
-  <si>
     <t>White as Snow</t>
   </si>
   <si>
@@ -555,9 +420,6 @@
     <t>Eric Altmayer / Nicolas Altmayer / Philippe Carcassonne</t>
   </si>
   <si>
-    <t>Anne Fontaine</t>
-  </si>
-  <si>
     <t>Baking Up Love</t>
   </si>
   <si>
@@ -570,12 +432,6 @@
     <t>Jeffrey L. Kaufman</t>
   </si>
   <si>
-    <t>Amy Minter / Jennifer Haniff Thompson</t>
-  </si>
-  <si>
-    <t>Candice T. Cain</t>
-  </si>
-  <si>
     <t>Naked Singularity</t>
   </si>
   <si>
@@ -588,12 +444,6 @@
     <t>Anna Boden / François Callens / Ryan Fleck / Tony Pachella / Sébastien Raybaud / Mark Roberts / Deborah Roth / Ridley Scott / Dick Wolf / John Zois</t>
   </si>
   <si>
-    <t>Susan Leber / Sam Roston</t>
-  </si>
-  <si>
-    <t>Chase Palmer</t>
-  </si>
-  <si>
     <t>The East</t>
   </si>
   <si>
@@ -603,10 +453,187 @@
     <t>Frank Klein / Aram Tertzakian</t>
   </si>
   <si>
-    <t>Philip Harthoorn</t>
-  </si>
-  <si>
-    <t>Jim Taihuttu</t>
+    <t>Shawn Levy ((directed by)) / Dan Cohen (co-producer) / Rand Geiger (co-producer)</t>
+  </si>
+  <si>
+    <t>Shawn Levy / Michael Riley McGrath / Josh McLaglen / Mary McLaglen / Ryan Reynolds / Sarah Schechter</t>
+  </si>
+  <si>
+    <t>James Gunn () / Arianne Benedetti (line producer: Panama unit) / Simon Hatt (co-producer) / Lars P. Winther (co-producer)</t>
+  </si>
+  <si>
+    <t>James Gunn / Arianne Benedetti / Walter Hamada / Simon Hatt / Nikolas Korda / Charles Roven / Peter Safran / Deborah Snyder / Zack Snyder / Richard Suckle / Chantal Nong Vo / Lars P. Winther</t>
+  </si>
+  <si>
+    <t>Nia DaCosta ((directed by)) / Brittany Klesic (co-producer)</t>
+  </si>
+  <si>
+    <t>Nia DaCosta / Shauna Bryan / Jason Cloth / Ian Cooper / Aaron L. Gilbert / Catherine Hughes / David Kern / Brittany Klesic / Daniel F. Larson / Jordan Peele / Win Rosenfeld</t>
+  </si>
+  <si>
+    <t>Cal Brunker ((directed by)) / Laura Clunie (co-producer) / Amanda Morgan Palmer (co-executive producer) / Toni Stevens (co-producer) / Lauren Talbot (line producer) / Laurence Vacher (line producer)</t>
+  </si>
+  <si>
+    <t>Cal Brunker / Bob Barlen / Adam Beder / Laura Clunie / Jennifer Dodge / Ronnen Harary / Zai Ortiz / Amanda Morgan Palmer / Peter Schlessel / Toni Stevens / Lauren Talbot / Laurence Vacher</t>
+  </si>
+  <si>
+    <t>Rodo Sayagues () / Romel Adam (co-producer) / Brady Fujikawa (co-producer) / Kelli Konop (co-producer) / Dave Krieger (line producer: Detroit) / Rodo Sayagues (co-producer)</t>
+  </si>
+  <si>
+    <t>Rodo Sayagues / Rob Tapert / Erin Westerman</t>
+  </si>
+  <si>
+    <t>Liesl Tommy ()</t>
+  </si>
+  <si>
+    <t>Martin Campbell ((directed by)) / Ekaterina Baker (co-executive producer) / Valentin Dimitrov (line producer: Bulgaria) / Bernard Mazauric (line producer) / Gabriel Popescu (line producer) / Lonnie Ramati (co-executive producer) / Regina Seifert (co-producer)</t>
+  </si>
+  <si>
+    <t>Martin Campbell / Ekaterina Baker / Andrei Boncea / Dragos Buliga / Christa Campbell / Luke Daniels / Boaz Davidson / Moshe Diamant / Valentin Dimitrov / Claiton Fernandes / Vladimir Fernandes / Jeffrey Greenstein / Lati Grobman / Eduard Irimia / Avi Lerner / Yariv Lerner / Bernard Mazauric / Balan Melarkode / Christopher Milburn / Euzebio Munhoz Jr. / Daniel Negret / Gabriel Popescu / Lonnie Ramati / Arthur Sarkissian / Regina Seifert / Trevor Short / Kyle Stroud / Robert Van Norden / Gareth West / Simon Williams / Bruno Wu / Jonathan Yunger</t>
+  </si>
+  <si>
+    <t>David Bruckner ((directed by)) / Alexander Norton (line producer: additional photography) / Todd Williams (consulting producer)</t>
+  </si>
+  <si>
+    <t>David Bruckner / François Callens / Ben Collins / Tara Finegan / David S. Goyer / Keith Levine / Alexander Norton / George Paaswell / Jeffrey Penman / Luke Piotrowski / Sébastien Raybaud / David Tracy / Todd Williams / Laura Wilson / John Zois</t>
+  </si>
+  <si>
+    <t>Lisa Joy ((directed by))</t>
+  </si>
+  <si>
+    <t>Lisa Joy / D. Scott Lumpkin / Jonathan Nolan / Aaron Ryder / Athena Wickham</t>
+  </si>
+  <si>
+    <t>Gabriel Riva Palacio Alatriste () / Rodolfo Riva Palacio Alatriste () / Paula Báez (production coordinator) / Regina Diaz Torre (line producer) / Estefanía Franco (coordinating producer) / Andy Rodríguez (assistant producer) / Janine Hernández Vidals (assistant producer) / María Sol Yépez (coordinating producer)</t>
+  </si>
+  <si>
+    <t>Gabriel Riva Palacio Alatriste / Rodolfo Riva Palacio Alatriste / Andy Rodríguez / Jd Segura Jr. / Cleo Segura Sherrel / Janine Hernández Vidals / María Sol Yépez / Carlos Zepeda</t>
+  </si>
+  <si>
+    <t>Sean Penn () / Mary Aloe (co-producer) / Gillian Hormel (co-producer) / Mark Montague (line producer) / Dana Mulligan (co-producer) / John Ira Palmer (co-producer) / Matt Palmieri (co-producer) / Joseph Sacks (co-producer) / Katheryn Winnick (co-producer)</t>
+  </si>
+  <si>
+    <t>Sean Penn / Mary Aloe / Michael Cho / Christelle Conan / William Horberg / Gillian Hormel / Jon Kilik / Lawrence M. Kopeikin / Phyllis Laing / Tim Lee / Mark Montague / Dana Mulligan / John Ira Palmer / Matt Palmieri / Joseph Sacks / Thorsten Schumacher / Fernando Sulichin / Peter Touche / Devan Towers / John Wildermuth / Katheryn Winnick</t>
+  </si>
+  <si>
+    <t>Andreas Koefoed () / Duska Zagorac (Story Producer)</t>
+  </si>
+  <si>
+    <t>Andreas Koefoed / Andreas Dalsgaard / Oli Harbottle / Christoph Jörg / Mark Mitten / Ken Pelletier / Kasper Lykke Schultz / Vijay Vaidyanathan / Duska Zagorac</t>
+  </si>
+  <si>
+    <t>Benny Chan ()</t>
+  </si>
+  <si>
+    <t>Benny Chan / Donnie Yen / Albert Yeung</t>
+  </si>
+  <si>
+    <t>Seung-wan Ryoo ((directed by))</t>
+  </si>
+  <si>
+    <t>Seung-wan Ryoo / Seong-min Jo / Jung-min Kim / Su-jin Park</t>
+  </si>
+  <si>
+    <t>Stephen Daldry () / Justin Martin ((co-director)) / Robert How (line producer (as Rob How))</t>
+  </si>
+  <si>
+    <t>Stephen Daldry / Justin Martin / Sonia Friedman / Rose Garnett / Guy Heeley / Gaynor Holmes / Robert How / Dennis Kelly</t>
+  </si>
+  <si>
+    <t>Todd Stephens () / Kenneth Altman (line producer)</t>
+  </si>
+  <si>
+    <t>Todd Stephens / Roshon Thomas / Rhet Topham / Jess Weiss</t>
+  </si>
+  <si>
+    <t>Neill Blomkamp ()</t>
+  </si>
+  <si>
+    <t>Neill Blomkamp / Alastair Burlingham / Charlie Dombek / Stuart Ford / Gary Lam / Linda McDonough / Viktor Muller / Miguel Palos / Steven St. Arnaud</t>
+  </si>
+  <si>
+    <t>Oren Jacoby () / Joel Goodman ()</t>
+  </si>
+  <si>
+    <t>Oren Jacoby / Joel Goodman</t>
+  </si>
+  <si>
+    <t>Autumn de Wilde () / Thea Paulett (creative executive: Working Title Films) / Katherine Pomfret (senior production executive: Working Title Films) / Jo Wallett (co-producer)</t>
+  </si>
+  <si>
+    <t>Autumn de Wilde / Tim Bevan / Graham Broadbent / Peter Czernin / Eric Fellner / Amelia Granger / Ben Knight / Thea Paulett / Katherine Pomfret / Jo Wallett</t>
+  </si>
+  <si>
+    <t>Glenn Danzig () / Charles Arthur Berg (consulting producer (as Charles Berg) / consulting producer)</t>
+  </si>
+  <si>
+    <t>Glenn Danzig / Jarrett Furst / Brian Perera / Yvonne Perera / Tim Yasui</t>
+  </si>
+  <si>
+    <t>Debbie Isitt () / May Chu (co-producer) / Nick Jones (co-producer / line producer)</t>
+  </si>
+  <si>
+    <t>Debbie Isitt / Ian Benson / May Chu / Oliver Edwards / Ian Flooks / Nick Jones / Joe Oppenheimer / Andrew Taylor / Lee Thomas / David M. Thompson</t>
+  </si>
+  <si>
+    <t>Dash Shaw ()</t>
+  </si>
+  <si>
+    <t>Dash Shaw / Dexter Braff / Tyler Davidson / Gail Flannigan / Kyle Martin / Jane Samborski / Drew Sykes / Bill Way / William G. Way</t>
+  </si>
+  <si>
+    <t>Marion Hill ()</t>
+  </si>
+  <si>
+    <t>Marion Hill / Ben Matheny / Kelsey Scult / Zaferhan Yumru</t>
+  </si>
+  <si>
+    <t>Pascual Sisto () / Rowan Riley (co-producer) / Sam Slater (co-producer) / Fernando Tsai (co-executive producer)</t>
+  </si>
+  <si>
+    <t>Pascual Sisto / Sam Slater / Fernando Tsai / Marco Vicini</t>
+  </si>
+  <si>
+    <t>Savannah Ostler () / Alison Arngrim (co-producer) / Mario DeAngelis (line producer) / Cal Nguyen (co-producer) / Monica Moore Smith (co-producer)</t>
+  </si>
+  <si>
+    <t>Savannah Ostler / Stephen Ostler / Gay Lynn Smith / Monica Moore Smith / Nathan Steve Smith / Theodore Stump</t>
+  </si>
+  <si>
+    <t>Lucy Walker () / Jennie Bedusa (co-producer) / Christine Connor (co-producer) / Sam Kahn (field producer)</t>
+  </si>
+  <si>
+    <t>Lucy Walker / Lynda Weinman / Jamie Wolf / Maria Zuckerman</t>
+  </si>
+  <si>
+    <t>Petra Epperlein () / Michael Tucker ()</t>
+  </si>
+  <si>
+    <t>Petra Epperlein / Marie Therese Guirgis / Mike Lerner / Jeffrey Lurie / Dana O'Keefe / Michael Tucker</t>
+  </si>
+  <si>
+    <t>Anne Fontaine ()</t>
+  </si>
+  <si>
+    <t>Anne Fontaine / Eric Altmayer / Nicolas Altmayer / Philippe Carcassonne</t>
+  </si>
+  <si>
+    <t>Candice T. Cain () / Amy Minter (line producer) / Jennifer Haniff Thompson (supervising producer)</t>
+  </si>
+  <si>
+    <t>Candice T. Cain / Paula D'Amico / Jeffrey L. Kaufman / Monika Mannix / Amy Minter / Jennifer Muccioli / Thomas Osborne / Jennifer Haniff Thompson / Jeff Timmons</t>
+  </si>
+  <si>
+    <t>Chase Palmer () / Susan Leber (line producer) / Sam Roston (co-producer)</t>
+  </si>
+  <si>
+    <t>Chase Palmer / Anna Boden / François Callens / P. Jennifer Dana / Ryan Fleck / Tony Ganz / Ross Jacobson / Susan Leber / Tony Pachella / Sébastien Raybaud / Mark Roberts / Sam Roston / Deborah Roth / Ridley Scott / Ryan Stowell / Kevin J. Walsh / Dick Wolf / John Zois</t>
+  </si>
+  <si>
+    <t>Jim Taihuttu () / Philip Harthoorn (line producer)</t>
+  </si>
+  <si>
+    <t>Jim Taihuttu / Shanty Harmayn / Philip Harthoorn / Frank Klein / Julius Ponten / Benoit Roland / Aram Tertzakian / Sander Verdonk</t>
   </si>
 </sst>
 </file>
@@ -614,7 +641,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -647,7 +674,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,9 +993,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1027,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1008,13 +1035,13 @@
         <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>109283832</v>
+        <v>109650198</v>
       </c>
       <c r="D2" s="1">
         <v>193600000</v>
       </c>
       <c r="E2" s="1">
-        <v>302883832</v>
+        <v>303250198</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1026,18 +1053,18 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>55570323</v>
@@ -1049,239 +1076,245 @@
         <v>166470323</v>
       </c>
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="C4" s="1">
+        <v>54076070</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E4" s="1">
+        <v>68883070</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1">
-        <v>53806045</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1">
-        <v>68613045</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
       <c r="C5" s="1">
-        <v>37387749</v>
+        <v>37522903</v>
       </c>
       <c r="D5" s="1">
         <v>66100000</v>
       </c>
       <c r="E5" s="1">
-        <v>103487749</v>
+        <v>103622903</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1">
-        <v>31471613</v>
+        <v>31529898</v>
       </c>
       <c r="D6" s="1">
         <v>14600000</v>
       </c>
       <c r="E6" s="1">
-        <v>46071613</v>
+        <v>46129898</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1">
-        <v>23829364</v>
+        <v>23867893</v>
       </c>
       <c r="D7" s="1">
         <v>5577000</v>
       </c>
       <c r="E7" s="1">
-        <v>29406364</v>
+        <v>29444893</v>
       </c>
       <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7440368</v>
+      </c>
+      <c r="D8" s="1">
+        <v>714349</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8154717</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6962656</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4823443</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11786099</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="I9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7433846</v>
-      </c>
-      <c r="D8" s="1">
-        <v>713547</v>
-      </c>
-      <c r="E8" s="1">
-        <v>8147393</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6953198</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4032633</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10985831</v>
-      </c>
-      <c r="F9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
         <v>3890043</v>
       </c>
       <c r="D10" s="1">
-        <v>15588853</v>
+        <v>15945112</v>
       </c>
       <c r="E10" s="1">
-        <v>19478896</v>
+        <v>19835155</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="I10" t="s">
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>893849</v>
@@ -1293,114 +1326,117 @@
         <v>3316644</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1">
-        <v>418372</v>
+        <v>419351</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1">
-        <v>418372</v>
+        <v>419351</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="J12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1">
         <v>381044</v>
       </c>
       <c r="D13" s="1">
-        <v>15542</v>
+        <v>19808</v>
       </c>
       <c r="E13" s="1">
-        <v>396586</v>
+        <v>400852</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="J13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1">
         <v>368301</v>
       </c>
       <c r="D14" s="1">
-        <v>197323912</v>
+        <v>197324772</v>
       </c>
       <c r="E14" s="1">
-        <v>197692213</v>
+        <v>197693073</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
+        <v>162</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1">
         <v>297482</v>
@@ -1412,79 +1448,82 @@
         <v>28334928</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
+        <v>164</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
-        <v>214107</v>
+        <v>214339</v>
       </c>
       <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1">
+        <v>214339</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="1">
-        <v>214107</v>
-      </c>
-      <c r="F16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" t="s">
-        <v>100</v>
-      </c>
       <c r="I16" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1">
         <v>122855</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1">
         <v>122855</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="J17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1">
         <v>71334</v>
@@ -1496,47 +1535,50 @@
         <v>155304</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>87</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1">
         <v>67923</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1">
         <v>67923</v>
       </c>
       <c r="I19" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="J19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1">
         <v>51676</v>
@@ -1548,256 +1590,265 @@
         <v>368889</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H20" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="J20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C21" s="1">
         <v>44736</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1">
         <v>44736</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="J21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1">
         <v>33500</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1">
         <v>33500</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="I22" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="J22" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1">
         <v>32338</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E23" s="1">
         <v>32338</v>
       </c>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="H23" t="s">
-        <v>141</v>
+        <v>105</v>
+      </c>
+      <c r="I23" t="s">
+        <v>180</v>
       </c>
       <c r="J23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1">
         <v>27271</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1">
         <v>27271</v>
       </c>
       <c r="F24" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>146</v>
+        <v>109</v>
+      </c>
+      <c r="I24" t="s">
+        <v>182</v>
       </c>
       <c r="J24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1">
         <v>25386</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1">
         <v>25386</v>
       </c>
       <c r="F25" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="H25" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="I25" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="J25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1">
         <v>15671</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1">
         <v>15671</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="G26" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="H26" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="J26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
         <v>13375</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1">
         <v>13375</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="G27" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="I27" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1">
         <v>12804</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1">
         <v>12804</v>
       </c>
       <c r="F28" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>168</v>
+        <v>124</v>
+      </c>
+      <c r="I28" t="s">
+        <v>190</v>
       </c>
       <c r="J28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="C29" s="1">
         <v>7881</v>
@@ -1809,76 +1860,79 @@
         <v>302591</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>127</v>
+      </c>
+      <c r="I29" t="s">
+        <v>192</v>
       </c>
       <c r="J29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1">
         <v>6286</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E30" s="1">
         <v>6286</v>
       </c>
       <c r="F30" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
       <c r="I30" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="J30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="C31" s="1">
         <v>3050</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E31" s="1">
         <v>3050</v>
       </c>
       <c r="F31" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="H31" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="I31" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="J31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1">
         <v>180</v>
@@ -1890,16 +1944,16 @@
         <v>160187</v>
       </c>
       <c r="F32" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="H32" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="I32" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="J32" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugged some selectors and made IMDB faster
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabh\Documents\UiPath\MovieSearch2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C171C848-35F3-4804-9192-81C179FF602F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86E57D3-001F-4B7F-910A-66BD4759C7FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11325" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="190">
   <si>
     <t>Movie Name</t>
   </si>
@@ -72,6 +72,255 @@
     <t>20th Century Studios</t>
   </si>
   <si>
+    <t>The Suicide Squad</t>
+  </si>
+  <si>
+    <t>Warner Bros.</t>
+  </si>
+  <si>
+    <t>Candyman</t>
+  </si>
+  <si>
+    <t>Universal Pictures</t>
+  </si>
+  <si>
+    <t>PAW Patrol: The Movie</t>
+  </si>
+  <si>
+    <t>Paramount Pictures</t>
+  </si>
+  <si>
+    <t>Don't Breathe 2</t>
+  </si>
+  <si>
+    <t>Screen Gems</t>
+  </si>
+  <si>
+    <t>Respect</t>
+  </si>
+  <si>
+    <t>Metro-Goldwyn-Mayer (MGM)</t>
+  </si>
+  <si>
+    <t>Liesl Tommy</t>
+  </si>
+  <si>
+    <t>The Protege</t>
+  </si>
+  <si>
+    <t>Lionsgate</t>
+  </si>
+  <si>
+    <t>The Night House</t>
+  </si>
+  <si>
+    <t>Searchlight Pictures</t>
+  </si>
+  <si>
+    <t>Reminiscence</t>
+  </si>
+  <si>
+    <t>An Egg Rescue</t>
+  </si>
+  <si>
+    <t>Pantelion Films</t>
+  </si>
+  <si>
+    <t>Flag Day</t>
+  </si>
+  <si>
+    <t>United Artists Releasing</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>The Lost Leonardo</t>
+  </si>
+  <si>
+    <t>Sony Pictures Classics</t>
+  </si>
+  <si>
+    <t>Raging Fire</t>
+  </si>
+  <si>
+    <t>Well Go USA Entertainment</t>
+  </si>
+  <si>
+    <t>Escape from Mogadishu</t>
+  </si>
+  <si>
+    <t>Together</t>
+  </si>
+  <si>
+    <t>Swan Song</t>
+  </si>
+  <si>
+    <t>Magnolia Pictures</t>
+  </si>
+  <si>
+    <t>Demonic</t>
+  </si>
+  <si>
+    <t>IFC Films</t>
+  </si>
+  <si>
+    <t>On Broadway</t>
+  </si>
+  <si>
+    <t>Kino Lorber</t>
+  </si>
+  <si>
+    <t>Ema</t>
+  </si>
+  <si>
+    <t>Music Box Films</t>
+  </si>
+  <si>
+    <t>Death Rider in the House of Vampires</t>
+  </si>
+  <si>
+    <t>Atlas Distribution Company</t>
+  </si>
+  <si>
+    <t>Confetti</t>
+  </si>
+  <si>
+    <t>Dada Films</t>
+  </si>
+  <si>
+    <t>Cryptozoo</t>
+  </si>
+  <si>
+    <t>Ma Belle, My Beauty</t>
+  </si>
+  <si>
+    <t>Good Deed Entertainment</t>
+  </si>
+  <si>
+    <t>John and the Hole</t>
+  </si>
+  <si>
+    <t>Even in Dreams</t>
+  </si>
+  <si>
+    <t>Purdie Distribution</t>
+  </si>
+  <si>
+    <t>Bring Your Own Brigade</t>
+  </si>
+  <si>
+    <t>The Meaning of Hitler</t>
+  </si>
+  <si>
+    <t>White as Snow</t>
+  </si>
+  <si>
+    <t>Cohen Media Group</t>
+  </si>
+  <si>
+    <t>Baking Up Love</t>
+  </si>
+  <si>
+    <t>Naked Singularity</t>
+  </si>
+  <si>
+    <t>Screen Media Films</t>
+  </si>
+  <si>
+    <t>The East</t>
+  </si>
+  <si>
+    <t>Shawn Levy</t>
+  </si>
+  <si>
+    <t>James Gunn</t>
+  </si>
+  <si>
+    <t>Nia DaCosta</t>
+  </si>
+  <si>
+    <t>Cal Brunker</t>
+  </si>
+  <si>
+    <t>Rodo Sayagues</t>
+  </si>
+  <si>
+    <t>Martin Campbell</t>
+  </si>
+  <si>
+    <t>David Bruckner</t>
+  </si>
+  <si>
+    <t>Lisa Joy</t>
+  </si>
+  <si>
+    <t>Gabriel Riva Palacio Alatriste / Rodolfo Riva Palacio Alatriste</t>
+  </si>
+  <si>
+    <t>Sean Penn</t>
+  </si>
+  <si>
+    <t>Andreas Koefoed</t>
+  </si>
+  <si>
+    <t>Benny Chan</t>
+  </si>
+  <si>
+    <t>Seung-wan Ryoo</t>
+  </si>
+  <si>
+    <t>Stephen Daldry / Justin Martin</t>
+  </si>
+  <si>
+    <t>Todd Stephens</t>
+  </si>
+  <si>
+    <t>Neill Blomkamp</t>
+  </si>
+  <si>
+    <t>Oren Jacoby</t>
+  </si>
+  <si>
+    <t>Autumn de Wilde</t>
+  </si>
+  <si>
+    <t>Glenn Danzig</t>
+  </si>
+  <si>
+    <t>Debbie Isitt</t>
+  </si>
+  <si>
+    <t>Dash Shaw</t>
+  </si>
+  <si>
+    <t>Marion Hill</t>
+  </si>
+  <si>
+    <t>Pascual Sisto</t>
+  </si>
+  <si>
+    <t>Savannah Ostler</t>
+  </si>
+  <si>
+    <t>Lucy Walker</t>
+  </si>
+  <si>
+    <t>Petra Epperlein / Michael Tucker</t>
+  </si>
+  <si>
+    <t>Anne Fontaine</t>
+  </si>
+  <si>
+    <t>Candice T. Cain</t>
+  </si>
+  <si>
+    <t>Chase Palmer</t>
+  </si>
+  <si>
+    <t>Jim Taihuttu</t>
+  </si>
+  <si>
     <t>Greg Berlanti / Adam Kolbrenner / Shawn Levy / Ryan Reynolds / Sarah Schechter</t>
   </si>
   <si>
@@ -81,10 +330,7 @@
     <t>George Dewey / Dan Levine / Michael Riley McGrath / Josh McLaglen / Mary McLaglen</t>
   </si>
   <si>
-    <t>The Suicide Squad</t>
-  </si>
-  <si>
-    <t>Warner Bros.</t>
+    <t>Dan Cohen (co-producer) / Rand Geiger (co-producer)</t>
   </si>
   <si>
     <t>Charles Roven / Peter Safran</t>
@@ -93,13 +339,7 @@
     <t>Walter Hamada / Nikolas Korda / Deborah Snyder / Zack Snyder / Richard Suckle / Chantal Nong Vo</t>
   </si>
   <si>
-    <t>Candyman</t>
-  </si>
-  <si>
-    <t>Universal Pictures</t>
-  </si>
-  <si>
-    <t>Crew information</t>
+    <t>Arianne Benedetti (line producer: Panama unit) / Simon Hatt (co-producer) / Lars P. Winther (co-producer)</t>
   </si>
   <si>
     <t>Ian Cooper / Jordan Peele / Win Rosenfeld</t>
@@ -111,10 +351,7 @@
     <t>Shauna Bryan / Jason Cloth / Aaron L. Gilbert / David Kern</t>
   </si>
   <si>
-    <t>PAW Patrol: The Movie</t>
-  </si>
-  <si>
-    <t>Paramount Pictures</t>
+    <t>Brittany Klesic (co-producer)</t>
   </si>
   <si>
     <t>Jennifer Dodge</t>
@@ -126,10 +363,7 @@
     <t>Adam Beder / Ronnen Harary / Zai Ortiz / Peter Schlessel</t>
   </si>
   <si>
-    <t>Don't Breathe 2</t>
-  </si>
-  <si>
-    <t>Screen Gems</t>
+    <t>Laura Clunie (co-producer) / Amanda Morgan Palmer (co-executive producer) / Toni Stevens (co-producer) / Lauren Talbot (line producer) / Laurence Vacher (line producer)</t>
   </si>
   <si>
     <t>Fede Alvarez / Sam Raimi / Rob Tapert</t>
@@ -141,10 +375,7 @@
     <t>Joseph Drake / Rick Jacobson / Nathan Kahane / Stephen Lang / Andrew Pfeffer / Erin Westerman</t>
   </si>
   <si>
-    <t>Respect</t>
-  </si>
-  <si>
-    <t>Metro-Goldwyn-Mayer (MGM)</t>
+    <t>Romel Adam (co-producer) / Brady Fujikawa (co-producer) / Kelli Konop (co-producer) / Dave Krieger (line producer: Detroit) / Rodo Sayagues (co-producer)</t>
   </si>
   <si>
     <t>Scott Bernstein / Jonathan Glickman / Harvey Mason Jr. / Stacey Sher</t>
@@ -153,15 +384,6 @@
     <t>Sue Baden-Powell / Jason Cloth / Aaron L. Gilbert / Jennifer Hudson / Liesl Tommy</t>
   </si>
   <si>
-    <t>Liesl Tommy</t>
-  </si>
-  <si>
-    <t>The Protege</t>
-  </si>
-  <si>
-    <t>Lionsgate</t>
-  </si>
-  <si>
     <t>Moshe Diamant / Yariv Lerner / Christopher Milburn / Arthur Sarkissian / Robert Van Norden</t>
   </si>
   <si>
@@ -171,10 +393,7 @@
     <t>Andrei Boncea / Dragos Buliga / Christa Campbell / Luke Daniels / Boaz Davidson / Claiton Fernandes / Vladimir Fernandes / Jeffrey Greenstein / Lati Grobman / Avi Lerner / Balan Melarkode / Euzebio Munhoz Jr. / Daniel Negret / Trevor Short / Kyle Stroud / Gareth West / Simon Williams / Bruno Wu / Jonathan Yunger</t>
   </si>
   <si>
-    <t>The Night House</t>
-  </si>
-  <si>
-    <t>Searchlight Pictures</t>
+    <t>Ekaterina Baker (co-executive producer) / Valentin Dimitrov (line producer: Bulgaria) / Bernard Mazauric (line producer) / Gabriel Popescu (line producer) / Lonnie Ramati (co-executive producer) / Regina Seifert (co-producer)</t>
   </si>
   <si>
     <t>David S. Goyer / Keith Levine / John Zois</t>
@@ -186,7 +405,7 @@
     <t>David Bruckner / François Callens / Ben Collins / Tara Finegan / George Paaswell / Luke Piotrowski / Sébastien Raybaud / Laura Wilson</t>
   </si>
   <si>
-    <t>Reminiscence</t>
+    <t>Alexander Norton (line producer: additional photography) / Todd Williams (consulting producer)</t>
   </si>
   <si>
     <t>Michael De Luca / Lisa Joy / Jonathan Nolan / Aaron Ryder</t>
@@ -198,25 +417,13 @@
     <t>Elishia Holmes / D. Scott Lumpkin / Athena Wickham</t>
   </si>
   <si>
-    <t>An Egg Rescue</t>
-  </si>
-  <si>
-    <t>Pantelion Films</t>
-  </si>
-  <si>
     <t>Ignacio Martínez Casares / Gabriel Riva Palacio Alatriste / Rodolfo Riva Palacio Alatriste</t>
   </si>
   <si>
     <t>Mineko Mori / Jd Segura Jr. / Cleo Segura Sherrel / Carlos Zepeda</t>
   </si>
   <si>
-    <t>Flag Day</t>
-  </si>
-  <si>
-    <t>United Artists Releasing</t>
-  </si>
-  <si>
-    <t>–</t>
+    <t>Paula Báez (production coordinator) / Regina Diaz Torre (line producer) / Estefanía Franco (coordinating producer) / Andy Rodríguez (assistant producer) / Janine Hernández Vidals (assistant producer) / María Sol Yépez (coordinating producer)</t>
   </si>
   <si>
     <t>William Horberg / Jon Kilik / Fernando Sulichin</t>
@@ -228,10 +435,7 @@
     <t>Christelle Conan / Lawrence M. Kopeikin / Phyllis Laing / Thorsten Schumacher / Peter Touche / Devan Towers / John Wildermuth</t>
   </si>
   <si>
-    <t>The Lost Leonardo</t>
-  </si>
-  <si>
-    <t>Sony Pictures Classics</t>
+    <t>Mary Aloe (co-producer) / Gillian Hormel (co-producer) / Mark Montague (line producer) / Dana Mulligan (co-producer) / John Ira Palmer (co-producer) / Matt Palmieri (co-producer) / Joseph Sacks (co-producer) / Katheryn Winnick (co-producer)</t>
   </si>
   <si>
     <t>Andreas Dalsgaard / Christoph Jörg</t>
@@ -243,10 +447,7 @@
     <t>Oli Harbottle / Mark Mitten / Ken Pelletier / Vijay Vaidyanathan</t>
   </si>
   <si>
-    <t>Raging Fire</t>
-  </si>
-  <si>
-    <t>Well Go USA Entertainment</t>
+    <t>Duska Zagorac (Story Producer)</t>
   </si>
   <si>
     <t>Benny Chan / Donnie Yen</t>
@@ -255,25 +456,16 @@
     <t>Albert Yeung</t>
   </si>
   <si>
-    <t>Escape from Mogadishu</t>
-  </si>
-  <si>
     <t>Seong-min Jo / Jung-min Kim / Su-jin Park</t>
   </si>
   <si>
-    <t>Together</t>
-  </si>
-  <si>
     <t>Sonia Friedman / Guy Heeley</t>
   </si>
   <si>
     <t>Rose Garnett / Gaynor Holmes / Dennis Kelly</t>
   </si>
   <si>
-    <t>Swan Song</t>
-  </si>
-  <si>
-    <t>Magnolia Pictures</t>
+    <t>Robert How (line producer (as Rob How))</t>
   </si>
   <si>
     <t>Eric Eisenbrey / Stephen Israel / Tim Kaltenecker / Todd Stephens</t>
@@ -285,10 +477,7 @@
     <t>Jay Michael Fraley / Drew Sklar / Rhet Topham</t>
   </si>
   <si>
-    <t>Demonic</t>
-  </si>
-  <si>
-    <t>IFC Films</t>
+    <t>Kenneth Altman (line producer)</t>
   </si>
   <si>
     <t>Mike Blomkamp / Neill Blomkamp / Stuart Ford / Linda McDonough</t>
@@ -300,28 +489,13 @@
     <t>Alastair Burlingham / Charlie Dombek / Viktor Muller / Miguel Palos / Steven St. Arnaud</t>
   </si>
   <si>
-    <t>On Broadway</t>
-  </si>
-  <si>
-    <t>Kino Lorber</t>
-  </si>
-  <si>
-    <t>Ema</t>
-  </si>
-  <si>
-    <t>Music Box Films</t>
-  </si>
-  <si>
     <t>Tim Bevan / Graham Broadbent / Peter Czernin / Eric Fellner</t>
   </si>
   <si>
     <t>Amelia Granger / Ben Knight</t>
   </si>
   <si>
-    <t>Death Rider in the House of Vampires</t>
-  </si>
-  <si>
-    <t>Atlas Distribution Company</t>
+    <t>Thea Paulett (creative executive: Working Title Films) / Katherine Pomfret (senior production executive: Working Title Films) / Jo Wallett (co-producer)</t>
   </si>
   <si>
     <t>James Cullen Bressack</t>
@@ -333,10 +507,7 @@
     <t>Glenn Danzig / Brian Perera / Yvonne Perera</t>
   </si>
   <si>
-    <t>Confetti</t>
-  </si>
-  <si>
-    <t>Dada Films</t>
+    <t>Charles Arthur Berg (consulting producer (as Charles Berg) / consulting producer)</t>
   </si>
   <si>
     <t>Ian Benson / Ian Flooks</t>
@@ -345,7 +516,7 @@
     <t>Oliver Edwards / Joe Oppenheimer / Andrew Taylor / Lee Thomas / David M. Thompson</t>
   </si>
   <si>
-    <t>Cryptozoo</t>
+    <t>May Chu (co-producer) / Nick Jones (co-producer / line producer)</t>
   </si>
   <si>
     <t>Tyler Davidson / Kyle Martin / Jane Samborski / Bill Way / William G. Way</t>
@@ -354,31 +525,19 @@
     <t>Dexter Braff / Gail Flannigan / Drew Sykes</t>
   </si>
   <si>
-    <t>Ma Belle, My Beauty</t>
-  </si>
-  <si>
-    <t>Good Deed Entertainment</t>
-  </si>
-  <si>
     <t>Marion Hill / Ben Matheny / Kelsey Scult</t>
   </si>
   <si>
     <t>Zaferhan Yumru</t>
   </si>
   <si>
-    <t>John and the Hole</t>
-  </si>
-  <si>
     <t>Michael Bowes / Nicolás Giacobone / Alex Orlovsky / Elika Portnoy</t>
   </si>
   <si>
     <t>P. Jennifer Dana / Phil Hoelting / Ross Jacobson / Tony Pachella / Mark Roberts / Pascual Sisto / Marco Vicini</t>
   </si>
   <si>
-    <t>Even in Dreams</t>
-  </si>
-  <si>
-    <t>Purdie Distribution</t>
+    <t>Rowan Riley (co-producer) / Sam Slater (co-producer) / Fernando Tsai (co-executive producer)</t>
   </si>
   <si>
     <t>Dallas Ashton / Sarah Kent</t>
@@ -390,7 +549,7 @@
     <t>Robbie Bryan / Steven D'Alo / Pete D'Arruda / Sessalie Daun / Lucas A. Ferrara / Jacob Joseph / Savannah Ostler / Theodore Stump</t>
   </si>
   <si>
-    <t>Bring Your Own Brigade</t>
+    <t>Alison Arngrim (co-producer) / Mario DeAngelis (line producer) / Cal Nguyen (co-producer) / Monica Moore Smith (co-producer)</t>
   </si>
   <si>
     <t>Holly Becker / Julian Cautherley / Lyn Davis Lear / Martha Eidsness Mitchell / Lucy Walker</t>
@@ -402,7 +561,7 @@
     <t>Bill Benenson / Laurie Benenson / Michael Bloom / Geralyn White Dreyfous / Kathryn Everett / Ryan Heller / Tony Hsieh / Jena King / Lisa Leingang / Adam Lewis / Melony Lewis / Bryn Mooser / Regina K. Scully / Lynda Weinman / Jamie Wolf / Maria Zuckerman</t>
   </si>
   <si>
-    <t>The Meaning of Hitler</t>
+    <t>Jennie Bedusa (co-producer) / Christine Connor (co-producer) / Sam Kahn (field producer)</t>
   </si>
   <si>
     <t>Petra Epperlein / Mike Lerner / Dana O'Keefe / Michael Tucker</t>
@@ -411,18 +570,9 @@
     <t>Anthony Dobkin / Marie Therese Guirgis / Jeffrey Lurie</t>
   </si>
   <si>
-    <t>White as Snow</t>
-  </si>
-  <si>
-    <t>Cohen Media Group</t>
-  </si>
-  <si>
     <t>Eric Altmayer / Nicolas Altmayer / Philippe Carcassonne</t>
   </si>
   <si>
-    <t>Baking Up Love</t>
-  </si>
-  <si>
     <t>Monika Mannix / Jeff Timmons</t>
   </si>
   <si>
@@ -432,10 +582,7 @@
     <t>Jeffrey L. Kaufman</t>
   </si>
   <si>
-    <t>Naked Singularity</t>
-  </si>
-  <si>
-    <t>Screen Media Films</t>
+    <t>Amy Minter (line producer) / Jennifer Haniff Thompson (supervising producer)</t>
   </si>
   <si>
     <t>P. Jennifer Dana / Tony Ganz / Ross Jacobson / Ryan Stowell / Kevin J. Walsh</t>
@@ -444,7 +591,7 @@
     <t>Anna Boden / François Callens / Ryan Fleck / Tony Pachella / Sébastien Raybaud / Mark Roberts / Deborah Roth / Ridley Scott / Dick Wolf / John Zois</t>
   </si>
   <si>
-    <t>The East</t>
+    <t>Susan Leber (line producer) / Sam Roston (co-producer)</t>
   </si>
   <si>
     <t>Shanty Harmayn / Julius Ponten / Benoit Roland / Sander Verdonk</t>
@@ -453,187 +600,10 @@
     <t>Frank Klein / Aram Tertzakian</t>
   </si>
   <si>
-    <t>Shawn Levy ((directed by)) / Dan Cohen (co-producer) / Rand Geiger (co-producer)</t>
-  </si>
-  <si>
-    <t>Shawn Levy / Michael Riley McGrath / Josh McLaglen / Mary McLaglen / Ryan Reynolds / Sarah Schechter</t>
-  </si>
-  <si>
-    <t>James Gunn () / Arianne Benedetti (line producer: Panama unit) / Simon Hatt (co-producer) / Lars P. Winther (co-producer)</t>
-  </si>
-  <si>
-    <t>James Gunn / Arianne Benedetti / Walter Hamada / Simon Hatt / Nikolas Korda / Charles Roven / Peter Safran / Deborah Snyder / Zack Snyder / Richard Suckle / Chantal Nong Vo / Lars P. Winther</t>
-  </si>
-  <si>
-    <t>Nia DaCosta ((directed by)) / Brittany Klesic (co-producer)</t>
-  </si>
-  <si>
-    <t>Nia DaCosta / Shauna Bryan / Jason Cloth / Ian Cooper / Aaron L. Gilbert / Catherine Hughes / David Kern / Brittany Klesic / Daniel F. Larson / Jordan Peele / Win Rosenfeld</t>
-  </si>
-  <si>
-    <t>Cal Brunker ((directed by)) / Laura Clunie (co-producer) / Amanda Morgan Palmer (co-executive producer) / Toni Stevens (co-producer) / Lauren Talbot (line producer) / Laurence Vacher (line producer)</t>
-  </si>
-  <si>
-    <t>Cal Brunker / Bob Barlen / Adam Beder / Laura Clunie / Jennifer Dodge / Ronnen Harary / Zai Ortiz / Amanda Morgan Palmer / Peter Schlessel / Toni Stevens / Lauren Talbot / Laurence Vacher</t>
-  </si>
-  <si>
-    <t>Rodo Sayagues () / Romel Adam (co-producer) / Brady Fujikawa (co-producer) / Kelli Konop (co-producer) / Dave Krieger (line producer: Detroit) / Rodo Sayagues (co-producer)</t>
-  </si>
-  <si>
-    <t>Rodo Sayagues / Rob Tapert / Erin Westerman</t>
-  </si>
-  <si>
-    <t>Liesl Tommy ()</t>
-  </si>
-  <si>
-    <t>Martin Campbell ((directed by)) / Ekaterina Baker (co-executive producer) / Valentin Dimitrov (line producer: Bulgaria) / Bernard Mazauric (line producer) / Gabriel Popescu (line producer) / Lonnie Ramati (co-executive producer) / Regina Seifert (co-producer)</t>
-  </si>
-  <si>
-    <t>Martin Campbell / Ekaterina Baker / Andrei Boncea / Dragos Buliga / Christa Campbell / Luke Daniels / Boaz Davidson / Moshe Diamant / Valentin Dimitrov / Claiton Fernandes / Vladimir Fernandes / Jeffrey Greenstein / Lati Grobman / Eduard Irimia / Avi Lerner / Yariv Lerner / Bernard Mazauric / Balan Melarkode / Christopher Milburn / Euzebio Munhoz Jr. / Daniel Negret / Gabriel Popescu / Lonnie Ramati / Arthur Sarkissian / Regina Seifert / Trevor Short / Kyle Stroud / Robert Van Norden / Gareth West / Simon Williams / Bruno Wu / Jonathan Yunger</t>
-  </si>
-  <si>
-    <t>David Bruckner ((directed by)) / Alexander Norton (line producer: additional photography) / Todd Williams (consulting producer)</t>
-  </si>
-  <si>
-    <t>David Bruckner / François Callens / Ben Collins / Tara Finegan / David S. Goyer / Keith Levine / Alexander Norton / George Paaswell / Jeffrey Penman / Luke Piotrowski / Sébastien Raybaud / David Tracy / Todd Williams / Laura Wilson / John Zois</t>
-  </si>
-  <si>
-    <t>Lisa Joy ((directed by))</t>
-  </si>
-  <si>
-    <t>Lisa Joy / D. Scott Lumpkin / Jonathan Nolan / Aaron Ryder / Athena Wickham</t>
-  </si>
-  <si>
-    <t>Gabriel Riva Palacio Alatriste () / Rodolfo Riva Palacio Alatriste () / Paula Báez (production coordinator) / Regina Diaz Torre (line producer) / Estefanía Franco (coordinating producer) / Andy Rodríguez (assistant producer) / Janine Hernández Vidals (assistant producer) / María Sol Yépez (coordinating producer)</t>
-  </si>
-  <si>
-    <t>Gabriel Riva Palacio Alatriste / Rodolfo Riva Palacio Alatriste / Andy Rodríguez / Jd Segura Jr. / Cleo Segura Sherrel / Janine Hernández Vidals / María Sol Yépez / Carlos Zepeda</t>
-  </si>
-  <si>
-    <t>Sean Penn () / Mary Aloe (co-producer) / Gillian Hormel (co-producer) / Mark Montague (line producer) / Dana Mulligan (co-producer) / John Ira Palmer (co-producer) / Matt Palmieri (co-producer) / Joseph Sacks (co-producer) / Katheryn Winnick (co-producer)</t>
-  </si>
-  <si>
-    <t>Sean Penn / Mary Aloe / Michael Cho / Christelle Conan / William Horberg / Gillian Hormel / Jon Kilik / Lawrence M. Kopeikin / Phyllis Laing / Tim Lee / Mark Montague / Dana Mulligan / John Ira Palmer / Matt Palmieri / Joseph Sacks / Thorsten Schumacher / Fernando Sulichin / Peter Touche / Devan Towers / John Wildermuth / Katheryn Winnick</t>
-  </si>
-  <si>
-    <t>Andreas Koefoed () / Duska Zagorac (Story Producer)</t>
-  </si>
-  <si>
-    <t>Andreas Koefoed / Andreas Dalsgaard / Oli Harbottle / Christoph Jörg / Mark Mitten / Ken Pelletier / Kasper Lykke Schultz / Vijay Vaidyanathan / Duska Zagorac</t>
-  </si>
-  <si>
-    <t>Benny Chan ()</t>
-  </si>
-  <si>
-    <t>Benny Chan / Donnie Yen / Albert Yeung</t>
-  </si>
-  <si>
-    <t>Seung-wan Ryoo ((directed by))</t>
-  </si>
-  <si>
-    <t>Seung-wan Ryoo / Seong-min Jo / Jung-min Kim / Su-jin Park</t>
-  </si>
-  <si>
-    <t>Stephen Daldry () / Justin Martin ((co-director)) / Robert How (line producer (as Rob How))</t>
-  </si>
-  <si>
-    <t>Stephen Daldry / Justin Martin / Sonia Friedman / Rose Garnett / Guy Heeley / Gaynor Holmes / Robert How / Dennis Kelly</t>
-  </si>
-  <si>
-    <t>Todd Stephens () / Kenneth Altman (line producer)</t>
-  </si>
-  <si>
-    <t>Todd Stephens / Roshon Thomas / Rhet Topham / Jess Weiss</t>
-  </si>
-  <si>
-    <t>Neill Blomkamp ()</t>
-  </si>
-  <si>
-    <t>Neill Blomkamp / Alastair Burlingham / Charlie Dombek / Stuart Ford / Gary Lam / Linda McDonough / Viktor Muller / Miguel Palos / Steven St. Arnaud</t>
-  </si>
-  <si>
-    <t>Oren Jacoby () / Joel Goodman ()</t>
-  </si>
-  <si>
-    <t>Oren Jacoby / Joel Goodman</t>
-  </si>
-  <si>
-    <t>Autumn de Wilde () / Thea Paulett (creative executive: Working Title Films) / Katherine Pomfret (senior production executive: Working Title Films) / Jo Wallett (co-producer)</t>
-  </si>
-  <si>
-    <t>Autumn de Wilde / Tim Bevan / Graham Broadbent / Peter Czernin / Eric Fellner / Amelia Granger / Ben Knight / Thea Paulett / Katherine Pomfret / Jo Wallett</t>
-  </si>
-  <si>
-    <t>Glenn Danzig () / Charles Arthur Berg (consulting producer (as Charles Berg) / consulting producer)</t>
-  </si>
-  <si>
-    <t>Glenn Danzig / Jarrett Furst / Brian Perera / Yvonne Perera / Tim Yasui</t>
-  </si>
-  <si>
-    <t>Debbie Isitt () / May Chu (co-producer) / Nick Jones (co-producer / line producer)</t>
-  </si>
-  <si>
-    <t>Debbie Isitt / Ian Benson / May Chu / Oliver Edwards / Ian Flooks / Nick Jones / Joe Oppenheimer / Andrew Taylor / Lee Thomas / David M. Thompson</t>
-  </si>
-  <si>
-    <t>Dash Shaw ()</t>
-  </si>
-  <si>
-    <t>Dash Shaw / Dexter Braff / Tyler Davidson / Gail Flannigan / Kyle Martin / Jane Samborski / Drew Sykes / Bill Way / William G. Way</t>
-  </si>
-  <si>
-    <t>Marion Hill ()</t>
-  </si>
-  <si>
-    <t>Marion Hill / Ben Matheny / Kelsey Scult / Zaferhan Yumru</t>
-  </si>
-  <si>
-    <t>Pascual Sisto () / Rowan Riley (co-producer) / Sam Slater (co-producer) / Fernando Tsai (co-executive producer)</t>
-  </si>
-  <si>
-    <t>Pascual Sisto / Sam Slater / Fernando Tsai / Marco Vicini</t>
-  </si>
-  <si>
-    <t>Savannah Ostler () / Alison Arngrim (co-producer) / Mario DeAngelis (line producer) / Cal Nguyen (co-producer) / Monica Moore Smith (co-producer)</t>
-  </si>
-  <si>
-    <t>Savannah Ostler / Stephen Ostler / Gay Lynn Smith / Monica Moore Smith / Nathan Steve Smith / Theodore Stump</t>
-  </si>
-  <si>
-    <t>Lucy Walker () / Jennie Bedusa (co-producer) / Christine Connor (co-producer) / Sam Kahn (field producer)</t>
-  </si>
-  <si>
-    <t>Lucy Walker / Lynda Weinman / Jamie Wolf / Maria Zuckerman</t>
-  </si>
-  <si>
-    <t>Petra Epperlein () / Michael Tucker ()</t>
-  </si>
-  <si>
-    <t>Petra Epperlein / Marie Therese Guirgis / Mike Lerner / Jeffrey Lurie / Dana O'Keefe / Michael Tucker</t>
-  </si>
-  <si>
-    <t>Anne Fontaine ()</t>
-  </si>
-  <si>
-    <t>Anne Fontaine / Eric Altmayer / Nicolas Altmayer / Philippe Carcassonne</t>
-  </si>
-  <si>
-    <t>Candice T. Cain () / Amy Minter (line producer) / Jennifer Haniff Thompson (supervising producer)</t>
-  </si>
-  <si>
-    <t>Candice T. Cain / Paula D'Amico / Jeffrey L. Kaufman / Monika Mannix / Amy Minter / Jennifer Muccioli / Thomas Osborne / Jennifer Haniff Thompson / Jeff Timmons</t>
-  </si>
-  <si>
-    <t>Chase Palmer () / Susan Leber (line producer) / Sam Roston (co-producer)</t>
-  </si>
-  <si>
-    <t>Chase Palmer / Anna Boden / François Callens / P. Jennifer Dana / Ryan Fleck / Tony Ganz / Ross Jacobson / Susan Leber / Tony Pachella / Sébastien Raybaud / Mark Roberts / Sam Roston / Deborah Roth / Ridley Scott / Ryan Stowell / Kevin J. Walsh / Dick Wolf / John Zois</t>
-  </si>
-  <si>
-    <t>Jim Taihuttu () / Philip Harthoorn (line producer)</t>
-  </si>
-  <si>
-    <t>Jim Taihuttu / Shanty Harmayn / Philip Harthoorn / Frank Klein / Julius Ponten / Benoit Roland / Aram Tertzakian / Sander Verdonk</t>
+    <t>Philip Harthoorn (line producer)</t>
+  </si>
+  <si>
+    <t>Joel Goodman</t>
   </si>
 </sst>
 </file>
@@ -672,8 +642,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -991,9 +962,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2793664-5744-4D0E-A5CB-621D09702C22}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="176" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="222.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1044,27 +1027,27 @@
         <v>303250198</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>55570323</v>
@@ -1076,56 +1059,56 @@
         <v>166470323</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="I3" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>54076070</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
+      <c r="D4" s="2">
+        <v>14807000</v>
       </c>
       <c r="E4" s="1">
         <v>68883070</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="J4" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>37522903</v>
@@ -1137,27 +1120,27 @@
         <v>103622903</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="J5" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>31529898</v>
@@ -1169,27 +1152,27 @@
         <v>46129898</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="I6" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>23867893</v>
@@ -1201,24 +1184,21 @@
         <v>29444893</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>7440368</v>
@@ -1230,27 +1210,27 @@
         <v>8154717</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="J8" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>6962656</v>
@@ -1262,27 +1242,27 @@
         <v>11786099</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>3890043</v>
@@ -1294,27 +1274,24 @@
         <v>19835155</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="J10" t="s">
-        <v>155</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1">
         <v>893849</v>
@@ -1326,56 +1303,56 @@
         <v>3316644</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="I11" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="J11" t="s">
-        <v>157</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1">
         <v>419351</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <v>419351</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="J12" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1">
         <v>381044</v>
@@ -1387,27 +1364,27 @@
         <v>400852</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="J13" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1">
         <v>368301</v>
@@ -1419,24 +1396,21 @@
         <v>197693073</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1">
         <v>297482</v>
@@ -1448,82 +1422,79 @@
         <v>28334928</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1">
         <v>214339</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
         <v>214339</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="I16" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="J16" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1">
         <v>122855</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1">
         <v>122855</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="I17" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="J17" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1">
         <v>71334</v>
@@ -1535,50 +1506,47 @@
         <v>155304</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1">
         <v>67923</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1">
         <v>67923</v>
       </c>
-      <c r="I19" t="s">
-        <v>172</v>
+      <c r="F19" t="s">
+        <v>189</v>
       </c>
       <c r="J19" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1">
         <v>51676</v>
@@ -1590,265 +1558,256 @@
         <v>368889</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="I20" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="J20" t="s">
-        <v>175</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>44736</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1">
         <v>44736</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="I21" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="J21" t="s">
-        <v>177</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
         <v>33500</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E22" s="1">
         <v>33500</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I22" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="J22" t="s">
-        <v>179</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>32338</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1">
         <v>32338</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="H23" t="s">
-        <v>105</v>
-      </c>
-      <c r="I23" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="J23" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1">
         <v>27271</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <v>27271</v>
       </c>
       <c r="F24" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="G24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="J24" t="s">
-        <v>183</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1">
         <v>25386</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1">
         <v>25386</v>
       </c>
       <c r="F25" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="H25" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="I25" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J25" t="s">
-        <v>185</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1">
         <v>15671</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1">
         <v>15671</v>
       </c>
       <c r="F26" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="H26" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="I26" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="J26" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
         <v>13375</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1">
         <v>13375</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="G27" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="H27" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="J27" t="s">
-        <v>189</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
         <v>12804</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1">
         <v>12804</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="H28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I28" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J28" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1">
         <v>7881</v>
@@ -1860,79 +1819,76 @@
         <v>302591</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
-      </c>
-      <c r="I29" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="J29" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1">
         <v>6286</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1">
         <v>6286</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="G30" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="I30" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J30" t="s">
-        <v>195</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1">
         <v>3050</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E31" s="1">
         <v>3050</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="H31" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="I31" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="J31" t="s">
-        <v>197</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1">
         <v>180</v>
@@ -1944,16 +1900,16 @@
         <v>160187</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="H32" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="I32" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="J32" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sorting and filtering for sheet 2
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabh\Documents\UiPath\MovieSearch2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will Zhang\Documents\UiPath\MovieSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D5965-A43F-4597-B545-FA45CFE06A5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DB61D1-5DB6-4A34-8156-7D2103070D0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
+    <workbookView minimized="1" xWindow="2498" yWindow="2123" windowWidth="34529" windowHeight="17407" activeTab="1" xr2:uid="{0F14E6BD-3F08-48DB-A5A3-991DF38F5A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="176">
   <si>
     <t>Movie Name</t>
   </si>
@@ -66,28 +67,28 @@
     <t>Directors</t>
   </si>
   <si>
+    <t>–</t>
+  </si>
+  <si>
     <t>Warner Bros.</t>
   </si>
   <si>
-    <t>–</t>
+    <t>Vertical Entertainment</t>
+  </si>
+  <si>
+    <t>Bleecker Street Media</t>
   </si>
   <si>
     <t>Sony Pictures Classics</t>
   </si>
   <si>
+    <t>IFC Films</t>
+  </si>
+  <si>
+    <t>RLJE Films</t>
+  </si>
+  <si>
     <t>Magnolia Pictures</t>
-  </si>
-  <si>
-    <t>IFC Films</t>
-  </si>
-  <si>
-    <t>Vertical Entertainment</t>
-  </si>
-  <si>
-    <t>Bleecker Street Media</t>
-  </si>
-  <si>
-    <t>RLJE Films</t>
   </si>
   <si>
     <t>Indican Pictures</t>
@@ -600,8 +601,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -610,7 +615,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -920,26 +946,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2793664-5744-4D0E-A5CB-621D09702C22}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="121" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="146.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="244.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="146.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="244.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +979,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -971,12 +998,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>46041123</v>
@@ -984,7 +1011,7 @@
       <c r="D2" s="1">
         <v>86800000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="8">
         <v>132841123</v>
       </c>
       <c r="F2" t="s">
@@ -997,12 +1024,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>5446607</v>
@@ -1010,7 +1037,7 @@
       <c r="D3" s="1">
         <v>1348748</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="8">
         <v>6795355</v>
       </c>
       <c r="F3" t="s">
@@ -1029,7 +1056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1040,10 +1067,10 @@
         <v>3110580</v>
       </c>
       <c r="D4" s="2">
-        <v>12255778</v>
-      </c>
-      <c r="E4" s="1">
-        <v>15366358</v>
+        <v>12257377</v>
+      </c>
+      <c r="E4" s="8">
+        <v>15367957</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -1055,7 +1082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1068,7 +1095,7 @@
       <c r="D5" s="1">
         <v>584851</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="8">
         <v>3162681</v>
       </c>
       <c r="F5" t="s">
@@ -1084,7 +1111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1095,10 +1122,10 @@
         <v>2143000</v>
       </c>
       <c r="D6" s="1">
-        <v>34475827</v>
-      </c>
-      <c r="E6" s="1">
-        <v>36618827</v>
+        <v>34613266</v>
+      </c>
+      <c r="E6" s="8">
+        <v>36756266</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -1110,21 +1137,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>2122771</v>
       </c>
       <c r="D7" s="1">
-        <v>20631766</v>
-      </c>
-      <c r="E7" s="1">
-        <v>22754537</v>
+        <v>20935553</v>
+      </c>
+      <c r="E7" s="8">
+        <v>23058324</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
@@ -1142,7 +1169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1155,7 +1182,7 @@
       <c r="D8" s="1">
         <v>6690494</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="8">
         <v>7527030</v>
       </c>
       <c r="F8" t="s">
@@ -1171,12 +1198,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1">
         <v>741895</v>
@@ -1184,7 +1211,7 @@
       <c r="D9" s="1">
         <v>814868</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="8">
         <v>1556763</v>
       </c>
       <c r="F9" t="s">
@@ -1200,7 +1227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1211,10 +1238,10 @@
         <v>418286</v>
       </c>
       <c r="D10" s="1">
-        <v>12734</v>
-      </c>
-      <c r="E10" s="1">
-        <v>431020</v>
+        <v>23786</v>
+      </c>
+      <c r="E10" s="8">
+        <v>442072</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
@@ -1232,7 +1259,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1245,7 +1272,7 @@
       <c r="D11" s="1">
         <v>694688</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="8">
         <v>1099426</v>
       </c>
       <c r="F11" t="s">
@@ -1261,12 +1288,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
         <v>282500</v>
@@ -1274,7 +1301,7 @@
       <c r="D12" s="3">
         <v>649516</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="8">
         <v>932016</v>
       </c>
       <c r="F12" t="s">
@@ -1293,7 +1320,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1306,7 +1333,7 @@
       <c r="D13" s="1">
         <v>550050</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="8">
         <v>723754</v>
       </c>
       <c r="F13" t="s">
@@ -1322,7 +1349,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1335,7 +1362,7 @@
       <c r="D14" s="1">
         <v>326266</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="8">
         <v>492266</v>
       </c>
       <c r="F14" t="s">
@@ -1354,7 +1381,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -1367,7 +1394,7 @@
       <c r="D15" s="1">
         <v>149963307</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="8">
         <v>150123320</v>
       </c>
       <c r="F15" t="s">
@@ -1380,12 +1407,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
         <v>143532</v>
@@ -1393,7 +1420,7 @@
       <c r="D16" s="4">
         <v>21684</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="8">
         <v>165216</v>
       </c>
       <c r="F16" t="s">
@@ -1409,12 +1436,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1">
         <v>116143</v>
@@ -1422,7 +1449,7 @@
       <c r="D17" s="3">
         <v>89735</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="8">
         <v>205878</v>
       </c>
       <c r="F17" t="s">
@@ -1441,12 +1468,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>95643</v>
@@ -1454,7 +1481,7 @@
       <c r="D18" s="1">
         <v>4680</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="8">
         <v>100323</v>
       </c>
       <c r="F18" t="s">
@@ -1470,7 +1497,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -1481,9 +1508,9 @@
         <v>52786</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8">
         <v>52786</v>
       </c>
       <c r="F19" t="s">
@@ -1499,7 +1526,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -1512,7 +1539,7 @@
       <c r="D20" s="1">
         <v>7735</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="8">
         <v>60468</v>
       </c>
       <c r="F20" t="s">
@@ -1528,12 +1555,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1">
         <v>50439</v>
@@ -1541,7 +1568,7 @@
       <c r="D21" s="3">
         <v>1107828</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="8">
         <v>1158267</v>
       </c>
       <c r="F21" t="s">
@@ -1560,20 +1587,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1">
         <v>39053</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8">
         <v>39053</v>
       </c>
       <c r="F22" t="s">
@@ -1592,7 +1619,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>139</v>
       </c>
@@ -1605,7 +1632,7 @@
       <c r="D23" s="4">
         <v>91792613</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="8">
         <v>91815762</v>
       </c>
       <c r="F23" t="s">
@@ -1615,7 +1642,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -1625,10 +1652,10 @@
       <c r="C24" s="1">
         <v>10368</v>
       </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="8">
         <v>10368</v>
       </c>
       <c r="F24" t="s">
@@ -1641,7 +1668,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -1651,10 +1678,10 @@
       <c r="C25" s="1">
         <v>6055</v>
       </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="8">
         <v>6055</v>
       </c>
       <c r="F25" t="s">
@@ -1670,12 +1697,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1">
         <v>5495</v>
@@ -1683,7 +1710,7 @@
       <c r="D26" s="4">
         <v>328671</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="8">
         <v>334166</v>
       </c>
       <c r="F26" t="s">
@@ -1699,20 +1726,20 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>156</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1">
         <v>4844</v>
       </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="8">
         <v>4844</v>
       </c>
       <c r="F27" t="s">
@@ -1722,20 +1749,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>159</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1">
         <v>2238</v>
       </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="8">
         <v>2238</v>
       </c>
       <c r="F28" t="s">
@@ -1751,7 +1778,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -1764,7 +1791,7 @@
       <c r="D29" s="1">
         <v>24374106</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="8">
         <v>24375211</v>
       </c>
       <c r="F29" t="s">
@@ -1783,17 +1810,17 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>170</v>
       </c>
       <c r="C30" s="1">
         <v>917</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="8">
         <v>917</v>
       </c>
       <c r="F30" t="s">
@@ -1812,16 +1839,441 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C34" s="8"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADBAC05-182D-4869-A978-1EF2E6908C2F}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.796875" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="8">
+        <v>150123320</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8">
+        <v>132841123</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="8">
+        <v>91815762</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="8">
+        <v>36756266</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="8">
+        <v>24375211</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="8">
+        <v>23058324</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8">
+        <v>15367957</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8">
+        <v>7527030</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6795355</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3162681</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1556763</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1158267</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1099426</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="8">
+        <v>932016</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="8">
+        <v>723754</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="8">
+        <v>492266</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="8">
+        <v>442072</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="8">
+        <v>334166</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="8">
+        <v>205878</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="8">
+        <v>165216</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="8">
+        <v>100323</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="8">
+        <v>60468</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="8">
+        <v>52786</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="8">
+        <v>39053</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="8">
+        <v>10368</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="8">
+        <v>6055</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="8">
+        <v>4844</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2238</v>
+      </c>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="8">
+        <v>917</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="E31" s="8"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J1:J31">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merged will's sorting branch
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylej\RPA_FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabh\Documents\UiPath\MovieSearch2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ACE170-21B5-4662-8E1A-71C222C0F374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602D88AB-45A8-4940-9B21-B889064F4AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="878" yWindow="1628" windowWidth="15390" windowHeight="9532" xr2:uid="{25EEE8E4-0EEA-4C78-B196-9C78A6541B9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{25EEE8E4-0EEA-4C78-B196-9C78A6541B9C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="195">
   <si>
     <t>Movie Name</t>
   </si>
@@ -618,15 +619,14 @@
     <t>For month:September</t>
   </si>
   <si>
-    <t>Ran at:10/04/2021 13:26:01</t>
+    <t>Collected at:10/04/2021 15:10:06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -662,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,20 +976,410 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500E8E2B-F83E-46E8-98A1-0AAD02E92CA2}">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>386908802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>30346326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>18215477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>11799160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>9857380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>6128006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>4999532</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>3265719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10">
+        <v>3252326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11">
+        <v>2101170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12">
+        <v>1909503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13">
+        <v>1754811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <v>931154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15">
+        <v>791483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>397824</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17">
+        <v>373169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>276961</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19">
+        <v>176993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20">
+        <v>133462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21">
+        <v>125254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22">
+        <v>110995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23">
+        <v>87513</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24">
+        <v>64968</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25">
+        <v>51351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26">
+        <v>35086</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27">
+        <v>33334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28">
+        <v>24778</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29">
+        <v>21515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30">
+        <v>15318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31">
+        <v>13028</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32">
+        <v>12245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33">
+        <v>11288</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34">
+        <v>2839</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4C5280-B4C2-48D8-B0E0-26F5D0ABB60A}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.9296875" customWidth="1"/>
-    <col min="3" max="3" width="29.46484375" customWidth="1"/>
-    <col min="4" max="4" width="22.86328125" customWidth="1"/>
-    <col min="5" max="5" width="22.9296875" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>194</v>
       </c>
@@ -997,7 +1387,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1087,859 +1477,859 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1">
+        <v>11799160</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
+        <v>11799160</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9144380</v>
+      </c>
+      <c r="D6" s="1">
+        <v>713000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9857380</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5001849</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1126157</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6128006</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2622730</v>
+      </c>
+      <c r="D8" s="1">
+        <v>642989</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3265719</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2101170</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2101170</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1754811</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1754811</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1">
+        <v>971000</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4028532</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4999532</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="1">
+        <v>780843</v>
+      </c>
+      <c r="D12" s="1">
+        <v>150311</v>
+      </c>
+      <c r="E12" s="1">
+        <v>931154</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1">
+        <v>738175</v>
+      </c>
+      <c r="D13" s="2">
+        <v>53308</v>
+      </c>
+      <c r="E13" s="1">
+        <v>791483</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C14" s="1">
         <v>428300</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D14" s="1">
         <v>17787177</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E14" s="1">
         <v>18215477</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H14" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I14" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1">
-        <v>11799160</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1">
+        <v>397824</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1">
-        <v>11799160</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9144380</v>
-      </c>
-      <c r="D7" s="1">
-        <v>713000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9857380</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5001849</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1126157</v>
-      </c>
-      <c r="E8" s="1">
-        <v>6128006</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1">
-        <v>971000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4028532</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4999532</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2622730</v>
-      </c>
-      <c r="D10" s="1">
-        <v>642989</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3265719</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="1">
-        <v>39540</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3212786</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3252326</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2101170</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E15" s="1">
+        <v>397824</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1">
+        <v>373169</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1">
-        <v>2101170</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1">
-        <v>21353</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1888150</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1909503</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1754811</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1754811</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="1">
-        <v>780843</v>
-      </c>
-      <c r="D15" s="1">
-        <v>150311</v>
-      </c>
-      <c r="E15" s="1">
-        <v>931154</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1">
-        <v>738175</v>
-      </c>
-      <c r="D16" s="2">
-        <v>53308</v>
-      </c>
       <c r="E16" s="1">
-        <v>791483</v>
+        <v>373169</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="C17" s="1">
-        <v>397824</v>
+        <v>110995</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="1">
-        <v>397824</v>
+        <v>110995</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="J17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1">
-        <v>373169</v>
-      </c>
-      <c r="D18" s="1" t="s">
+        <v>93564</v>
+      </c>
+      <c r="D18" s="1">
+        <v>183397</v>
+      </c>
+      <c r="E18" s="1">
+        <v>276961</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="1">
+        <v>87513</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1">
-        <v>373169</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" t="s">
-        <v>97</v>
-      </c>
-      <c r="J18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="1">
-        <v>93564</v>
-      </c>
-      <c r="D19" s="1">
-        <v>183397</v>
-      </c>
       <c r="E19" s="1">
-        <v>276961</v>
+        <v>87513</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
+      </c>
+      <c r="G19" t="s">
+        <v>131</v>
       </c>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C20" s="1">
-        <v>14667</v>
-      </c>
-      <c r="D20" s="1">
-        <v>162326</v>
+        <v>64968</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E20" s="1">
-        <v>176993</v>
+        <v>64968</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" t="s">
-        <v>108</v>
+        <v>137</v>
+      </c>
+      <c r="H20" t="s">
+        <v>138</v>
+      </c>
+      <c r="I20" t="s">
+        <v>139</v>
       </c>
       <c r="J20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C21" s="1">
-        <v>5095</v>
+        <v>51469</v>
       </c>
       <c r="D21" s="1">
-        <v>128367</v>
+        <v>73785</v>
       </c>
       <c r="E21" s="1">
-        <v>133462</v>
+        <v>125254</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="G21" t="s">
+        <v>118</v>
       </c>
       <c r="H21" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="I21" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="J21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="C22" s="1">
-        <v>51469</v>
+        <v>48516</v>
       </c>
       <c r="D22" s="2">
-        <v>73785</v>
+        <v>2835</v>
       </c>
       <c r="E22" s="1">
-        <v>125254</v>
+        <v>51351</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="I22" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="J22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1">
-        <v>110995</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>39540</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3212786</v>
       </c>
       <c r="E23" s="1">
-        <v>110995</v>
+        <v>3252326</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" t="s">
-        <v>124</v>
-      </c>
-      <c r="H23" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="J23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="C24" s="1">
-        <v>87513</v>
+        <v>35086</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="1">
-        <v>87513</v>
+        <v>35086</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G24" t="s">
-        <v>131</v>
-      </c>
-      <c r="H24" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="I24" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="J24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1">
-        <v>64968</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>29</v>
+        <v>29695</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3639</v>
       </c>
       <c r="E25" s="1">
-        <v>64968</v>
+        <v>33334</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="H25" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="I25" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="J25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="B26" t="s">
         <v>142</v>
       </c>
       <c r="C26" s="1">
-        <v>48516</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2835</v>
+        <v>21515</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E26" s="1">
-        <v>51351</v>
+        <v>21515</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I26" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="J26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1">
-        <v>35086</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>29</v>
+        <v>21353</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1888150</v>
       </c>
       <c r="E27" s="1">
-        <v>35086</v>
+        <v>1909503</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="I27" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="J27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1">
-        <v>29695</v>
+        <v>14667</v>
       </c>
       <c r="D28" s="1">
-        <v>3639</v>
+        <v>162326</v>
       </c>
       <c r="E28" s="1">
-        <v>33334</v>
+        <v>176993</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H28" t="s">
-        <v>155</v>
-      </c>
-      <c r="I28" t="s">
-        <v>156</v>
+        <v>107</v>
+      </c>
+      <c r="G28" t="s">
+        <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C29" s="1">
-        <v>6678</v>
+        <v>13589</v>
       </c>
       <c r="D29" s="2">
-        <v>18100</v>
+        <v>1729</v>
       </c>
       <c r="E29" s="1">
-        <v>24778</v>
+        <v>15318</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
+      </c>
+      <c r="G29" t="s">
+        <v>168</v>
       </c>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="I29" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="C30" s="1">
-        <v>21515</v>
+        <v>13028</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="1">
-        <v>21515</v>
+        <v>13028</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="J30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="C31" s="1">
-        <v>13589</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1729</v>
+        <v>12245</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E31" s="1">
-        <v>15318</v>
+        <v>12245</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G31" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H31" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I31" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>182</v>
+      </c>
+      <c r="B32" t="s">
+        <v>183</v>
       </c>
       <c r="C32" s="1">
-        <v>13028</v>
+        <v>11288</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E32" s="1">
-        <v>13028</v>
+        <v>11288</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>173</v>
+        <v>184</v>
+      </c>
+      <c r="G32" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" t="s">
+        <v>186</v>
+      </c>
+      <c r="I32" t="s">
+        <v>187</v>
       </c>
       <c r="J32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C33" s="1">
-        <v>12245</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>29</v>
+        <v>6678</v>
+      </c>
+      <c r="D33" s="2">
+        <v>18100</v>
       </c>
       <c r="E33" s="1">
-        <v>12245</v>
+        <v>24778</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G33" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="H33" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="I33" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="J33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="C34" s="1">
-        <v>11288</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>29</v>
+        <v>5095</v>
+      </c>
+      <c r="D34" s="2">
+        <v>128367</v>
       </c>
       <c r="E34" s="1">
-        <v>11288</v>
+        <v>133462</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G34" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="H34" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="I34" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="J34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
Kyle and Prabh - Added Exception handling for most of the cases, Testing OK.
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabh\Documents\UiPath\MovieSearch2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Part 4 SOFTENG\762\MovieSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1452D9F4-668C-4201-A618-B8E60A670046}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8AF1AE-CCCB-4816-8F29-A7764DC881D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="3705" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{25EEE8E4-0EEA-4C78-B196-9C78A6541B9C}"/>
+    <workbookView xWindow="2610" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{25EEE8E4-0EEA-4C78-B196-9C78A6541B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranked" sheetId="2" r:id="rId1"/>
@@ -35,9 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
-  <si>
-    <t>Collected at:10/05/2021 22:04:31</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="105">
+  <si>
+    <t>Collected at:10/16/2021 23:08:46</t>
   </si>
   <si>
     <t>For month:October</t>
@@ -91,40 +91,124 @@
     <t>Andy Serkis</t>
   </si>
   <si>
+    <t>No Time to Die</t>
+  </si>
+  <si>
+    <t>Metro-Goldwyn-Mayer (MGM)</t>
+  </si>
+  <si>
+    <t>Barbara Broccoli / Michael G. Wilson</t>
+  </si>
+  <si>
+    <t>Gregg Wilson</t>
+  </si>
+  <si>
+    <t>Chris Brigham</t>
+  </si>
+  <si>
+    <t>Per Henry Borch (line producer: Norway) / Daniel Craig (co-producer) / Andrew Noakes (co-producer) / David Pope (co-producer) / Enzo Sisti (line producer: italy) / Natalie Thompson (line producer: jamaica)</t>
+  </si>
+  <si>
+    <t>Cary Joji Fukunaga</t>
+  </si>
+  <si>
     <t>The Addams Family 2</t>
   </si>
   <si>
     <t>United Artists Releasing</t>
   </si>
   <si>
+    <t>Gail Berman / Alison O'Brien / Danielle Sterling / Conrad Vernon</t>
+  </si>
+  <si>
+    <t>Jason Cloth / Aaron L. Gilbert / Jonathan Glickman / Cassidy Lange / Kevin Miserocchi / Andrew Mittman</t>
+  </si>
+  <si>
+    <t>Barbara Zelinski (line producer)</t>
+  </si>
+  <si>
+    <t>Greg Tiernan / Conrad Vernon / Laura Brousseau / Kevin Pavlovic</t>
+  </si>
+  <si>
+    <t>The Many Saints of Newark</t>
+  </si>
+  <si>
+    <t>Warner Bros.</t>
+  </si>
+  <si>
+    <t>David Chase / Lawrence Konner / Nicole Lambert</t>
+  </si>
+  <si>
+    <t>Richard Brener / Michael Disco / Toby Emmerich / Marcus Viscidi</t>
+  </si>
+  <si>
+    <t>Alan Taylor</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>Piodor Gustafsson / Hrönn Kristinsdóttir / Sara Nassim / Jan Naszewski / Erik Rydell / Klaudia Smieja</t>
+  </si>
+  <si>
+    <t>Alicja Grawon / Helgi Jóhannsson / Marcin Luczaj</t>
+  </si>
+  <si>
+    <t>Marcin Drabinski / Jon Mankell / Håkan Pettersson / Peter Possne / Noomi Rapace / Béla Tarr</t>
+  </si>
+  <si>
+    <t>Zuzanna Hencz (co-producer)</t>
+  </si>
+  <si>
+    <t>Valdimar Jóhannsson</t>
+  </si>
+  <si>
+    <t>Titane</t>
+  </si>
+  <si>
+    <t>Neon</t>
+  </si>
+  <si>
+    <t>Jean-Christophe Reymond</t>
+  </si>
+  <si>
+    <t>Philippe Logie</t>
+  </si>
+  <si>
+    <t>Christophe Hollebeke</t>
+  </si>
+  <si>
+    <t>Anne-Laure Declerck (assistant producer) / Olivier Père (co-producer) / Jean-Yves Roubin (co-producer) / Cassandre Warnauts (co-producer)</t>
+  </si>
+  <si>
+    <t>Julia Ducournau</t>
+  </si>
+  <si>
+    <t>The Jesus Music</t>
+  </si>
+  <si>
+    <t>Lionsgate</t>
+  </si>
+  <si>
     <t>–</t>
   </si>
   <si>
-    <t>Gail Berman / Alison O'Brien / Danielle Sterling / Conrad Vernon</t>
-  </si>
-  <si>
-    <t>Jason Cloth / Aaron L. Gilbert / Jonathan Glickman / Cassidy Lange / Kevin Miserocchi / Andrew Mittman</t>
-  </si>
-  <si>
-    <t>Barbara Zelinski (line producer)</t>
-  </si>
-  <si>
-    <t>Greg Tiernan / Conrad Vernon / Laura Brousseau / Kevin Pavlovic</t>
-  </si>
-  <si>
-    <t>The Many Saints of Newark</t>
-  </si>
-  <si>
-    <t>Warner Bros.</t>
-  </si>
-  <si>
-    <t>David Chase / Lawrence Konner / Nicole Lambert</t>
-  </si>
-  <si>
-    <t>Richard Brener / Michael Disco / Toby Emmerich / Marcus Viscidi</t>
-  </si>
-  <si>
-    <t>Alan Taylor</t>
+    <t>Brandon Gregory / Josh Walsh</t>
+  </si>
+  <si>
+    <t>Katelyn Botsch</t>
+  </si>
+  <si>
+    <t>Kevin Downes / Andrew Erwin / Jon Erwin / Amy Grant / Greg Ham / Bill Reeves / Michael W. Smith / Tony Young</t>
+  </si>
+  <si>
+    <t>Parker Adams (co-producer) / Kyle Benn (co-producer) / Ben Field (co-producer) / Bekah Hubbell (Story Producer) / Kristopher Kimlin (co-producer) / Brian Mitchell (co-executive producer) / Ryan Whitaker (Story Producer) / Ben Woods (co-producer)</t>
+  </si>
+  <si>
+    <t>Andrew Erwin / Jon Erwin</t>
   </si>
   <si>
     <t>Chal Mera Putt 3</t>
@@ -139,43 +223,10 @@
     <t>Janjot Singh</t>
   </si>
   <si>
-    <t>The Jesus Music</t>
-  </si>
-  <si>
-    <t>Lionsgate</t>
-  </si>
-  <si>
-    <t>Brandon Gregory / Josh Walsh</t>
-  </si>
-  <si>
-    <t>Kevin Downes / Andrew Erwin / Jon Erwin / Amy Grant / Greg Ham / Bill Reeves / Michael W. Smith / Tony Young</t>
-  </si>
-  <si>
-    <t>Parker Adams (co-producer) / Kyle Benn (co-producer) / Ben Field (co-producer) / Bekah Hubbell (Story Producer) / Kristopher Kimlin (co-producer) / Ryan Whitaker (Story Producer) / Ben Woods (co-producer)</t>
-  </si>
-  <si>
-    <t>Andrew Erwin / Jon Erwin</t>
-  </si>
-  <si>
-    <t>Titane</t>
-  </si>
-  <si>
-    <t>Neon</t>
-  </si>
-  <si>
-    <t>Jean-Christophe Reymond</t>
-  </si>
-  <si>
-    <t>Philippe Logie</t>
-  </si>
-  <si>
-    <t>Christophe Hollebeke</t>
-  </si>
-  <si>
-    <t>Anne-Laure Declerck (assistant producer) / Olivier Père (co-producer) / Jean-Yves Roubin (co-producer) / Cassandre Warnauts (co-producer)</t>
-  </si>
-  <si>
-    <t>Julia Ducournau</t>
+    <t>Met Opera: Boris Godunov</t>
+  </si>
+  <si>
+    <t>Fathom Events</t>
   </si>
   <si>
     <t>Old Henry</t>
@@ -199,6 +250,21 @@
     <t>Potsy Ponciroli</t>
   </si>
   <si>
+    <t>Falling for Figaro</t>
+  </si>
+  <si>
+    <t>IFC Films</t>
+  </si>
+  <si>
+    <t>Judi Levine / Arabella Page Croft / Philip Wade</t>
+  </si>
+  <si>
+    <t>Charles Hannah / Donall McCusker / Kieran Parker / John Wade / Timothy White</t>
+  </si>
+  <si>
+    <t>Ben Lewin</t>
+  </si>
+  <si>
     <t>Possession</t>
   </si>
   <si>
@@ -211,19 +277,58 @@
     <t>Andrzej Zulawski</t>
   </si>
   <si>
-    <t>Falling for Figaro</t>
-  </si>
-  <si>
-    <t>IFC Films</t>
-  </si>
-  <si>
-    <t>Judi Levine / Arabella Page Croft / Philip Wade</t>
-  </si>
-  <si>
-    <t>Charles Hannah / Donall McCusker / Kieran Parker / John Wade / Timothy White</t>
-  </si>
-  <si>
-    <t>Ben Lewin</t>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Bleecker Street Media</t>
+  </si>
+  <si>
+    <t>Fran Kranz / Dylan Matlock / Casey Wilder Mott / J.P. Ouellette</t>
+  </si>
+  <si>
+    <t>Joe Abrams / Nico Falls / Douglas Matejka / Marshall Rawlings</t>
+  </si>
+  <si>
+    <t>Tony Becerra (co-producer) / William Thomas Andrew Davies (co-producer) / J. Davis (consulting producer) / Marissa Ghavami (co-producer)</t>
+  </si>
+  <si>
+    <t>Fran Kranz</t>
+  </si>
+  <si>
+    <t>Golden Voices</t>
+  </si>
+  <si>
+    <t>Music Box Films</t>
+  </si>
+  <si>
+    <t>Leon Edery / Moshe Edery / Eitan Evan / Tami Leon / Chilik Michaeli / Avraham Pirchi</t>
+  </si>
+  <si>
+    <t>Michal Wintroib (line producer)</t>
+  </si>
+  <si>
+    <t>Evgeny Ruman</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>MTV Documentary Films</t>
+  </si>
+  <si>
+    <t>Ronald Gilbert</t>
+  </si>
+  <si>
+    <t>Samantha Ellison / Matt Varosky</t>
+  </si>
+  <si>
+    <t>Jason Blum / Brett Burlock / Tim Gamble / Philip Levens / Mark Stern / Matthew Kaplan</t>
+  </si>
+  <si>
+    <t>Gary Evans (co-producer / associate producer (3 episodes, 2014)) / Ric Nish (co-producer (2 episodes, 2014))</t>
+  </si>
+  <si>
+    <t>Mairzee Almas / Nick Copus / Robert Lieberman / Vincenzo Natali / Stephen Williams</t>
   </si>
   <si>
     <t>Mayday</t>
@@ -244,7 +349,7 @@
     <t>Karen Cinorre</t>
   </si>
   <si>
-    <t>Collected at:10/05/2021 22:04:33</t>
+    <t>Collected at:10/16/2021 23:08:47</t>
   </si>
 </sst>
 </file>
@@ -614,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500E8E2B-F83E-46E8-98A1-0AAD02E92CA2}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +734,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -651,41 +756,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4">
-        <v>103833210</v>
+        <v>334238554</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4">
-        <v>17325007</v>
+        <v>195477670</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4">
-        <v>6951571</v>
+        <v>41004263</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -693,58 +798,58 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4">
-        <v>3065641</v>
+        <v>10848308</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4">
-        <v>1284809</v>
+        <v>3997208</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C8" s="4">
-        <v>548848</v>
+        <v>2021248</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4">
-        <v>21161</v>
+        <v>1496422</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,41 +857,122 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4">
-        <v>17000</v>
+        <v>953470</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
       <c r="C11" s="4">
-        <v>14335</v>
+        <v>574167</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4">
-        <v>3660</v>
+        <v>37194</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="4">
+        <v>30803</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="4">
+        <v>28312</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="4">
+        <v>24232</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4">
+        <v>21429</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8365</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4382</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -798,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4C5280-B4C2-48D8-B0E0-26F5D0ABB60A}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,13 +1049,13 @@
         <v>13</v>
       </c>
       <c r="C3" s="5">
-        <v>90033210</v>
+        <v>151577670</v>
       </c>
       <c r="D3" s="5">
-        <v>13800000</v>
-      </c>
-      <c r="E3">
-        <v>103833210</v>
+        <v>43900000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>195477670</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -892,15 +1078,18 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>17325007</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>75210554</v>
+      </c>
+      <c r="D4" s="1">
+        <v>259028000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>334238554</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1">
-        <v>17325007</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
       <c r="H4" t="s">
@@ -921,13 +1110,13 @@
         <v>26</v>
       </c>
       <c r="C5" s="1">
-        <v>4651571</v>
+        <v>35078263</v>
       </c>
       <c r="D5" s="1">
-        <v>2300000</v>
+        <v>5926000</v>
       </c>
       <c r="E5" s="1">
-        <v>6951571</v>
+        <v>41004263</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>27</v>
@@ -935,319 +1124,452 @@
       <c r="H5" t="s">
         <v>28</v>
       </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>644000</v>
+        <v>7938103</v>
       </c>
       <c r="D6" s="1">
-        <v>640809</v>
+        <v>2910205</v>
       </c>
       <c r="E6" s="1">
-        <v>1284809</v>
+        <v>10848308</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1">
-        <v>548848</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>1494726</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1696</v>
       </c>
       <c r="E7" s="1">
-        <v>548848</v>
+        <v>1496422</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1">
-        <v>533397</v>
+        <v>1207488</v>
       </c>
       <c r="D8" s="1">
-        <v>2532244</v>
+        <v>2789720</v>
       </c>
       <c r="E8" s="1">
-        <v>3065641</v>
+        <v>3997208</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1">
-        <v>21161</v>
+        <v>953470</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1">
-        <v>21161</v>
+        <v>953470</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1">
-        <v>17000</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>644000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1377248</v>
       </c>
       <c r="E10" s="1">
-        <v>17000</v>
+        <v>2021248</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1">
-        <v>14335</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>387000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>187167</v>
       </c>
       <c r="E11" s="1">
-        <v>14335</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
+        <v>574167</v>
+      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1">
-        <v>3660</v>
+        <v>37194</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1">
-        <v>3660</v>
+        <v>37194</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1">
+        <v>30803</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30803</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="1">
+        <v>24232</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1">
+        <v>24232</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="1">
+        <v>21429</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="1">
+        <v>21429</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9905</v>
+      </c>
+      <c r="D16" s="1">
+        <v>18407</v>
+      </c>
+      <c r="E16" s="1">
+        <v>28312</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8365</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8365</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4382</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4382</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>

</xml_diff>

<commit_message>
Added Year to the exported info
</commit_message>
<xml_diff>
--- a/ExportMovies.xlsx
+++ b/ExportMovies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Part 4 SOFTENG\762\MovieSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8AF1AE-CCCB-4816-8F29-A7764DC881D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DD0535-FCB7-4BD4-98F4-9BA3D67DD125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{25EEE8E4-0EEA-4C78-B196-9C78A6541B9C}"/>
   </bookViews>
@@ -35,12 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="105">
-  <si>
-    <t>Collected at:10/16/2021 23:08:46</t>
-  </si>
-  <si>
-    <t>For month:October</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
+  <si>
+    <t>Collected at:10/17/2021 16:56:55</t>
+  </si>
+  <si>
+    <t>For month:October, 2021</t>
   </si>
   <si>
     <t>Movie Name</t>
@@ -130,6 +130,30 @@
     <t>Greg Tiernan / Conrad Vernon / Laura Brousseau / Kevin Pavlovic</t>
   </si>
   <si>
+    <t>Halloween Kills</t>
+  </si>
+  <si>
+    <t>Universal Pictures</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>Malek Akkad / Bill Block / Jason Blum</t>
+  </si>
+  <si>
+    <t>Laura Altmann / Scott Clackum</t>
+  </si>
+  <si>
+    <t>John Carpenter / Jamie Lee Curtis / Ryan Freimann / Andrew Golov / David Gordon Green / Danny McBride / Bob Osher / Couper Samuelson / Jeanette Volturno</t>
+  </si>
+  <si>
+    <t>Sean Gowrie (co-producer) / Rick Osako (co-producer (as Rick A. Osako)) / Ryan Turek (co-producer) / Atilla Salih Yücer (co-producer)</t>
+  </si>
+  <si>
+    <t>David Gordon Green</t>
+  </si>
+  <si>
     <t>The Many Saints of Newark</t>
   </si>
   <si>
@@ -145,6 +169,27 @@
     <t>Alan Taylor</t>
   </si>
   <si>
+    <t>The Last Duel</t>
+  </si>
+  <si>
+    <t>Twentieth Century Fox</t>
+  </si>
+  <si>
+    <t>Ben Affleck / Matt Damon / Jennifer Fox / Nicole Holofcener / Ridley Scott / Kevin J. Walsh</t>
+  </si>
+  <si>
+    <t>Sasha Veneziano</t>
+  </si>
+  <si>
+    <t>Madison Ainley / Kevin Halloran / Drew Vinton</t>
+  </si>
+  <si>
+    <t>Aidan Elliott (co-producer) / James Flynn (producer: Metropolitan Films)</t>
+  </si>
+  <si>
+    <t>Ridley Scott</t>
+  </si>
+  <si>
     <t>Lamb</t>
   </si>
   <si>
@@ -193,9 +238,6 @@
     <t>Lionsgate</t>
   </si>
   <si>
-    <t>–</t>
-  </si>
-  <si>
     <t>Brandon Gregory / Josh Walsh</t>
   </si>
   <si>
@@ -349,7 +391,7 @@
     <t>Karen Cinorre</t>
   </si>
   <si>
-    <t>Collected at:10/16/2021 23:08:47</t>
+    <t>Collected at:10/17/2021 16:56:56</t>
   </si>
 </sst>
 </file>
@@ -719,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500E8E2B-F83E-46E8-98A1-0AAD02E92CA2}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="A1:XFD1048576"/>
@@ -734,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -762,7 +804,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="4">
-        <v>334238554</v>
+        <v>341446249</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -776,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="4">
-        <v>195477670</v>
+        <v>200057670</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -790,7 +832,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="4">
-        <v>41004263</v>
+        <v>42896524</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -798,13 +840,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="4">
-        <v>10848308</v>
+        <v>22800000</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -812,27 +854,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4">
-        <v>3997208</v>
+        <v>10848308</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="4">
-        <v>2021248</v>
+        <v>3997208</v>
       </c>
       <c r="D8" t="s">
         <v>59</v>
@@ -840,139 +882,167 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4">
-        <v>1496422</v>
+        <v>2021248</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1863000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="4">
-        <v>953470</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
       <c r="C11" s="4">
-        <v>574167</v>
+        <v>1668557</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4">
-        <v>37194</v>
+        <v>953470</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>75</v>
-      </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4">
-        <v>30803</v>
+        <v>574167</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4">
-        <v>28312</v>
+        <v>37194</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4">
-        <v>24232</v>
+        <v>30803</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C16" s="4">
-        <v>21429</v>
+        <v>28312</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="4">
+        <v>24232</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
-      </c>
-      <c r="C17" s="4">
-        <v>8365</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" s="4">
+        <v>21429</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8365</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="4">
         <v>4382</v>
       </c>
-      <c r="D18" t="s">
-        <v>99</v>
+      <c r="D20" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1049,13 +1119,13 @@
         <v>13</v>
       </c>
       <c r="C3" s="5">
-        <v>151577670</v>
+        <v>156157670</v>
       </c>
       <c r="D3" s="5">
         <v>43900000</v>
       </c>
       <c r="E3" s="5">
-        <v>195477670</v>
+        <v>200057670</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -1078,13 +1148,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>75210554</v>
+        <v>82418249</v>
       </c>
       <c r="D4" s="1">
         <v>259028000</v>
       </c>
       <c r="E4" s="1">
-        <v>334238554</v>
+        <v>341446249</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
@@ -1110,13 +1180,13 @@
         <v>26</v>
       </c>
       <c r="C5" s="1">
-        <v>35078263</v>
+        <v>36970524</v>
       </c>
       <c r="D5" s="1">
         <v>5926000</v>
       </c>
       <c r="E5" s="1">
-        <v>41004263</v>
+        <v>42896524</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>27</v>
@@ -1139,103 +1209,103 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>7938103</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2910205</v>
+        <v>22800000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="1">
-        <v>10848308</v>
+        <v>22800000</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
-        <v>1494726</v>
+        <v>7938103</v>
       </c>
       <c r="D7" s="2">
-        <v>1696</v>
+        <v>2910205</v>
       </c>
       <c r="E7" s="1">
-        <v>1496422</v>
+        <v>10848308</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1">
-        <v>1207488</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2789720</v>
+        <v>1863000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="1">
-        <v>3997208</v>
+        <v>1863000</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
-        <v>953470</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>1666861</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1696</v>
       </c>
       <c r="E9" s="1">
-        <v>953470</v>
+        <v>1668557</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>53</v>
@@ -1261,247 +1331,299 @@
         <v>59</v>
       </c>
       <c r="C10" s="1">
-        <v>644000</v>
+        <v>1207488</v>
       </c>
       <c r="D10" s="1">
-        <v>1377248</v>
+        <v>2789720</v>
       </c>
       <c r="E10" s="1">
-        <v>2021248</v>
+        <v>3997208</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1">
-        <v>387000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>187167</v>
+        <v>953470</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E11" s="1">
-        <v>574167</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>953470</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1">
-        <v>37194</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>644000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1377248</v>
       </c>
       <c r="E12" s="1">
-        <v>37194</v>
+        <v>2021248</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1">
-        <v>30803</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>387000</v>
+      </c>
+      <c r="D13" s="2">
+        <v>187167</v>
       </c>
       <c r="E13" s="1">
-        <v>30803</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" t="s">
-        <v>75</v>
-      </c>
+        <v>574167</v>
+      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1">
-        <v>24232</v>
+        <v>37194</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1">
-        <v>24232</v>
+        <v>37194</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1">
-        <v>21429</v>
+        <v>30803</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1">
-        <v>21429</v>
+        <v>30803</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1">
-        <v>9905</v>
-      </c>
-      <c r="D16" s="1">
-        <v>18407</v>
+        <v>24232</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="1">
-        <v>28312</v>
+        <v>24232</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J16" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1">
-        <v>8365</v>
+        <v>21429</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1">
-        <v>8365</v>
+        <v>21429</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1">
+        <v>9905</v>
+      </c>
+      <c r="D18" s="2">
+        <v>18407</v>
+      </c>
+      <c r="E18" s="1">
+        <v>28312</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8365</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1">
+        <v>8365</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="1">
         <v>4382</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1">
         <v>4382</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>

</xml_diff>